<commit_message>
- Wrapped up first version of the Campanian - Some issues with D47 reference frame were solved
</commit_message>
<xml_diff>
--- a/Campanian case/Kristianstad_raw_data.xlsx
+++ b/Campanian case/Kristianstad_raw_data.xlsx
@@ -8,14 +8,27 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nwi213\Dropbox\Research\Side projects\Bayesian temperature models\Seasonal DA\SeasonalDA_script\Campanian case\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{54481679-7785-403C-A669-B76F2BA9780A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83C3A5F6-BB09-4EB2-90DC-74B0CBA3ED7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{9382E40B-D560-4B2B-A771-AE95EF978F67}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{9382E40B-D560-4B2B-A771-AE95EF978F67}"/>
   </bookViews>
   <sheets>
     <sheet name="Kristianstad_raw_data" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -1651,7 +1664,7 @@
           <c:spPr>
             <a:ln w="19050" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent1"/>
+                <a:schemeClr val="accent2"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -1712,40 +1725,40 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="337"/>
                 <c:pt idx="0">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>18</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>0</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="7">
                   <c:v>5</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="8">
                   <c:v>5</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="9">
                   <c:v>6</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="10">
                   <c:v>19</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="11">
                   <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>18</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1774,7 +1787,7 @@
           <c:spPr>
             <a:ln w="19050" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent2"/>
+                <a:schemeClr val="accent5"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -1835,40 +1848,40 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="337"/>
                 <c:pt idx="0">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>11</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="6">
                   <c:v>1</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="7">
                   <c:v>2</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="8">
                   <c:v>0</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="9">
                   <c:v>2</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="10">
                   <c:v>4</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="11">
                   <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>17</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>28</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>14</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>20</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>16</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1958,40 +1971,40 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="337"/>
                 <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>13</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="6">
                   <c:v>12</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="7">
                   <c:v>13</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="8">
                   <c:v>6</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="9">
                   <c:v>0</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="10">
                   <c:v>6</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="11">
                   <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>19</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3339,14 +3352,14 @@
     <xdr:from>
       <xdr:col>10</xdr:col>
       <xdr:colOff>285750</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>90487</xdr:rowOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>33337</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
       <xdr:colOff>590550</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>166687</xdr:rowOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>109537</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3731,8 +3744,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0365049-C131-46D2-94F1-C2B0B50A8F70}">
   <dimension ref="A1:T339"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="X17" sqref="X17"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="W24" sqref="W24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3804,8 +3817,8 @@
         <v>0.16986301400000001</v>
       </c>
       <c r="J2">
-        <f>IF(A2="R. diluvianum", I2, IF(A2="A. incurva", MOD(I2-4/12, 1), MOD(I2-1/12, 1)))</f>
-        <v>0.16986301400000001</v>
+        <f>IF(A2="R. diluvianum", MOD(I2+5/12, 1), IF(A2="A. incurva", MOD(I2+1/12, 1), MOD(I2+4/12, 1)))</f>
+        <v>0.58652968066666666</v>
       </c>
       <c r="L2" t="s">
         <v>102</v>
@@ -3864,8 +3877,8 @@
         <v>0.16986301400000001</v>
       </c>
       <c r="J3">
-        <f t="shared" ref="J3:J66" si="0">IF(A3="R. diluvianum", I3, IF(A3="A. incurva", MOD(I3-4/12, 1), MOD(I3-1/12, 1)))</f>
-        <v>0.16986301400000001</v>
+        <f t="shared" ref="J3:J66" si="0">IF(A3="R. diluvianum", MOD(I3+5/12, 1), IF(A3="A. incurva", MOD(I3+1/12, 1), MOD(I3+4/12, 1)))</f>
+        <v>0.58652968066666666</v>
       </c>
       <c r="L3">
         <v>1</v>
@@ -3878,28 +3891,28 @@
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="O3">
-        <f>COUNTIFS(A:A,"=R. diluvianum",I:I,"&lt;"&amp;N3,I:I,"&gt;="&amp;M3)</f>
+        <f t="shared" ref="O3:O14" si="1">COUNTIFS(A:A,"=R. diluvianum",I:I,"&lt;"&amp;N3,I:I,"&gt;="&amp;M3)</f>
         <v>18</v>
       </c>
       <c r="P3">
-        <f>COUNTIFS(A:A,"=A. incurva",I:I,"&lt;"&amp;N3,I:I,"&gt;="&amp;M3)</f>
+        <f t="shared" ref="P3:P14" si="2">COUNTIFS(A:A,"=A. incurva",I:I,"&lt;"&amp;N3,I:I,"&gt;="&amp;M3)</f>
         <v>28</v>
       </c>
       <c r="Q3">
-        <f>COUNTIFS(A:A,"=B. suecicus",I:I,"&lt;"&amp;N3,I:I,"&gt;="&amp;M3)</f>
+        <f t="shared" ref="Q3:Q14" si="3">COUNTIFS(A:A,"=B. suecicus",I:I,"&lt;"&amp;N3,I:I,"&gt;="&amp;M3)</f>
         <v>19</v>
       </c>
       <c r="R3">
         <f>COUNTIFS(A:A,"=R. diluvianum",J:J,"&lt;"&amp;N3,J:J,"&gt;="&amp;M3)</f>
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="S3">
         <f>COUNTIFS(A:A,"=A. incurva",J:J,"&lt;"&amp;N3,J:J,"&gt;="&amp;M3)</f>
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="T3">
         <f>COUNTIFS(A:A,"=B. suecicus",J:J,"&lt;"&amp;N3,J:J,"&gt;="&amp;M3)</f>
-        <v>13</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
@@ -3932,7 +3945,7 @@
       </c>
       <c r="J4">
         <f t="shared" si="0"/>
-        <v>0.99726027399999995</v>
+        <v>0.41392694066666658</v>
       </c>
       <c r="L4">
         <v>2</v>
@@ -3946,28 +3959,28 @@
         <v>0.16666666666666666</v>
       </c>
       <c r="O4">
-        <f>COUNTIFS(A:A,"=R. diluvianum",I:I,"&lt;"&amp;N4,I:I,"&gt;="&amp;M4)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="P4">
-        <f>COUNTIFS(A:A,"=A. incurva",I:I,"&lt;"&amp;N4,I:I,"&gt;="&amp;M4)</f>
+        <f t="shared" si="2"/>
         <v>14</v>
       </c>
       <c r="Q4">
-        <f>COUNTIFS(A:A,"=B. suecicus",I:I,"&lt;"&amp;N4,I:I,"&gt;="&amp;M4)</f>
+        <f t="shared" si="3"/>
         <v>13</v>
       </c>
       <c r="R4">
-        <f t="shared" ref="R4:R14" si="1">COUNTIFS(A:A,"=R. diluvianum",J:J,"&lt;"&amp;N4,J:J,"&gt;="&amp;M4)</f>
-        <v>0</v>
+        <f t="shared" ref="R4:R14" si="4">COUNTIFS(A:A,"=R. diluvianum",J:J,"&lt;"&amp;N4,J:J,"&gt;="&amp;M4)</f>
+        <v>18</v>
       </c>
       <c r="S4">
-        <f t="shared" ref="S4:S14" si="2">COUNTIFS(A:A,"=A. incurva",J:J,"&lt;"&amp;N4,J:J,"&gt;="&amp;M4)</f>
-        <v>1</v>
+        <f t="shared" ref="S4:S14" si="5">COUNTIFS(A:A,"=A. incurva",J:J,"&lt;"&amp;N4,J:J,"&gt;="&amp;M4)</f>
+        <v>28</v>
       </c>
       <c r="T4">
-        <f t="shared" ref="T4:T14" si="3">COUNTIFS(A:A,"=B. suecicus",J:J,"&lt;"&amp;N4,J:J,"&gt;="&amp;M4)</f>
-        <v>12</v>
+        <f t="shared" ref="T4:T14" si="6">COUNTIFS(A:A,"=B. suecicus",J:J,"&lt;"&amp;N4,J:J,"&gt;="&amp;M4)</f>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">
@@ -4000,7 +4013,7 @@
       </c>
       <c r="J5">
         <f t="shared" si="0"/>
-        <v>0.99726027399999995</v>
+        <v>0.41392694066666658</v>
       </c>
       <c r="L5">
         <v>3</v>
@@ -4010,32 +4023,32 @@
         <v>0.16666666666666666</v>
       </c>
       <c r="N5">
-        <f>N4+N$3</f>
+        <f t="shared" ref="N5:N14" si="7">N4+N$3</f>
         <v>0.25</v>
       </c>
       <c r="O5">
-        <f>COUNTIFS(A:A,"=R. diluvianum",I:I,"&lt;"&amp;N5,I:I,"&gt;="&amp;M5)</f>
-        <v>5</v>
-      </c>
-      <c r="P5">
-        <f>COUNTIFS(A:A,"=A. incurva",I:I,"&lt;"&amp;N5,I:I,"&gt;="&amp;M5)</f>
-        <v>20</v>
-      </c>
-      <c r="Q5">
-        <f>COUNTIFS(A:A,"=B. suecicus",I:I,"&lt;"&amp;N5,I:I,"&gt;="&amp;M5)</f>
-        <v>12</v>
-      </c>
-      <c r="R5">
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
+      <c r="P5">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="Q5">
+        <f t="shared" si="3"/>
+        <v>12</v>
+      </c>
+      <c r="R5">
+        <f t="shared" si="4"/>
+        <v>10</v>
+      </c>
       <c r="S5">
-        <f t="shared" si="2"/>
-        <v>2</v>
+        <f t="shared" si="5"/>
+        <v>14</v>
       </c>
       <c r="T5">
-        <f t="shared" si="3"/>
-        <v>13</v>
+        <f t="shared" si="6"/>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
@@ -4068,42 +4081,42 @@
       </c>
       <c r="J6">
         <f t="shared" si="0"/>
-        <v>0.90410958900000005</v>
+        <v>0.32077625566666668</v>
       </c>
       <c r="L6">
         <v>4</v>
       </c>
       <c r="M6">
-        <f>M5+M$4</f>
+        <f t="shared" ref="M6:M14" si="8">M5+M$4</f>
         <v>0.25</v>
       </c>
       <c r="N6">
-        <f>N5+N$3</f>
+        <f t="shared" si="7"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="O6">
-        <f>COUNTIFS(A:A,"=R. diluvianum",I:I,"&lt;"&amp;N6,I:I,"&gt;="&amp;M6)</f>
-        <v>5</v>
-      </c>
-      <c r="P6">
-        <f>COUNTIFS(A:A,"=A. incurva",I:I,"&lt;"&amp;N6,I:I,"&gt;="&amp;M6)</f>
-        <v>16</v>
-      </c>
-      <c r="Q6">
-        <f>COUNTIFS(A:A,"=B. suecicus",I:I,"&lt;"&amp;N6,I:I,"&gt;="&amp;M6)</f>
-        <v>13</v>
-      </c>
-      <c r="R6">
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
+      <c r="P6">
+        <f t="shared" si="2"/>
+        <v>16</v>
+      </c>
+      <c r="Q6">
+        <f t="shared" si="3"/>
+        <v>13</v>
+      </c>
+      <c r="R6">
+        <f t="shared" si="4"/>
+        <v>8</v>
+      </c>
       <c r="S6">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <f t="shared" si="5"/>
+        <v>20</v>
       </c>
       <c r="T6">
-        <f t="shared" si="3"/>
-        <v>6</v>
+        <f t="shared" si="6"/>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.25">
@@ -4136,42 +4149,42 @@
       </c>
       <c r="J7">
         <f t="shared" si="0"/>
-        <v>0.90410958900000005</v>
+        <v>0.32077625566666668</v>
       </c>
       <c r="L7">
         <v>5</v>
       </c>
       <c r="M7">
-        <f>M6+M$4</f>
+        <f t="shared" si="8"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="N7">
-        <f>N6+N$3</f>
+        <f t="shared" si="7"/>
         <v>0.41666666666666663</v>
       </c>
       <c r="O7">
-        <f>COUNTIFS(A:A,"=R. diluvianum",I:I,"&lt;"&amp;N7,I:I,"&gt;="&amp;M7)</f>
-        <v>6</v>
-      </c>
-      <c r="P7">
-        <f>COUNTIFS(A:A,"=A. incurva",I:I,"&lt;"&amp;N7,I:I,"&gt;="&amp;M7)</f>
-        <v>11</v>
-      </c>
-      <c r="Q7">
-        <f>COUNTIFS(A:A,"=B. suecicus",I:I,"&lt;"&amp;N7,I:I,"&gt;="&amp;M7)</f>
-        <v>6</v>
-      </c>
-      <c r="R7">
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
+      <c r="P7">
+        <f t="shared" si="2"/>
+        <v>11</v>
+      </c>
+      <c r="Q7">
+        <f t="shared" si="3"/>
+        <v>6</v>
+      </c>
+      <c r="R7">
+        <f t="shared" si="4"/>
+        <v>4</v>
+      </c>
       <c r="S7">
-        <f t="shared" si="2"/>
-        <v>2</v>
+        <f t="shared" si="5"/>
+        <v>16</v>
       </c>
       <c r="T7">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <f t="shared" si="6"/>
+        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.25">
@@ -4204,42 +4217,42 @@
       </c>
       <c r="J8">
         <f t="shared" si="0"/>
-        <v>0.80547945200000004</v>
+        <v>0.22214611866666667</v>
       </c>
       <c r="L8">
         <v>6</v>
       </c>
       <c r="M8">
-        <f>M7+M$4</f>
+        <f t="shared" si="8"/>
         <v>0.41666666666666663</v>
       </c>
       <c r="N8">
-        <f>N7+N$3</f>
+        <f t="shared" si="7"/>
         <v>0.49999999999999994</v>
       </c>
       <c r="O8">
-        <f>COUNTIFS(A:A,"=R. diluvianum",I:I,"&lt;"&amp;N8,I:I,"&gt;="&amp;M8)</f>
-        <v>19</v>
-      </c>
-      <c r="P8">
-        <f>COUNTIFS(A:A,"=A. incurva",I:I,"&lt;"&amp;N8,I:I,"&gt;="&amp;M8)</f>
-        <v>1</v>
-      </c>
-      <c r="Q8">
-        <f>COUNTIFS(A:A,"=B. suecicus",I:I,"&lt;"&amp;N8,I:I,"&gt;="&amp;M8)</f>
-        <v>0</v>
-      </c>
-      <c r="R8">
         <f t="shared" si="1"/>
         <v>19</v>
       </c>
+      <c r="P8">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="Q8">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="R8">
+        <f t="shared" si="4"/>
+        <v>18</v>
+      </c>
       <c r="S8">
-        <f t="shared" si="2"/>
-        <v>4</v>
+        <f t="shared" si="5"/>
+        <v>11</v>
       </c>
       <c r="T8">
-        <f t="shared" si="3"/>
-        <v>6</v>
+        <f t="shared" si="6"/>
+        <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.25">
@@ -4272,42 +4285,42 @@
       </c>
       <c r="J9">
         <f t="shared" si="0"/>
-        <v>0.80547945200000004</v>
+        <v>0.22214611866666667</v>
       </c>
       <c r="L9">
         <v>7</v>
       </c>
       <c r="M9">
-        <f>M8+M$4</f>
+        <f t="shared" si="8"/>
         <v>0.49999999999999994</v>
       </c>
       <c r="N9">
-        <f>N8+N$3</f>
+        <f t="shared" si="7"/>
         <v>0.58333333333333326</v>
       </c>
       <c r="O9">
-        <f>COUNTIFS(A:A,"=R. diluvianum",I:I,"&lt;"&amp;N9,I:I,"&gt;="&amp;M9)</f>
-        <v>16</v>
-      </c>
-      <c r="P9">
-        <f>COUNTIFS(A:A,"=A. incurva",I:I,"&lt;"&amp;N9,I:I,"&gt;="&amp;M9)</f>
-        <v>2</v>
-      </c>
-      <c r="Q9">
-        <f>COUNTIFS(A:A,"=B. suecicus",I:I,"&lt;"&amp;N9,I:I,"&gt;="&amp;M9)</f>
-        <v>6</v>
-      </c>
-      <c r="R9">
         <f t="shared" si="1"/>
         <v>16</v>
       </c>
+      <c r="P9">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="Q9">
+        <f t="shared" si="3"/>
+        <v>6</v>
+      </c>
+      <c r="R9">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
       <c r="S9">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <f t="shared" si="5"/>
+        <v>1</v>
       </c>
       <c r="T9">
-        <f t="shared" si="3"/>
-        <v>9</v>
+        <f t="shared" si="6"/>
+        <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.25">
@@ -4340,42 +4353,42 @@
       </c>
       <c r="J10">
         <f t="shared" si="0"/>
-        <v>0.80547945200000004</v>
+        <v>0.22214611866666667</v>
       </c>
       <c r="L10">
         <v>8</v>
       </c>
       <c r="M10">
-        <f>M9+M$4</f>
+        <f t="shared" si="8"/>
         <v>0.58333333333333326</v>
       </c>
       <c r="N10">
-        <f>N9+N$3</f>
+        <f t="shared" si="7"/>
         <v>0.66666666666666663</v>
       </c>
       <c r="O10">
-        <f>COUNTIFS(A:A,"=R. diluvianum",I:I,"&lt;"&amp;N10,I:I,"&gt;="&amp;M10)</f>
-        <v>12</v>
-      </c>
-      <c r="P10">
-        <f>COUNTIFS(A:A,"=A. incurva",I:I,"&lt;"&amp;N10,I:I,"&gt;="&amp;M10)</f>
-        <v>0</v>
-      </c>
-      <c r="Q10">
-        <f>COUNTIFS(A:A,"=B. suecicus",I:I,"&lt;"&amp;N10,I:I,"&gt;="&amp;M10)</f>
-        <v>9</v>
-      </c>
-      <c r="R10">
         <f t="shared" si="1"/>
         <v>12</v>
       </c>
+      <c r="P10">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Q10">
+        <f t="shared" si="3"/>
+        <v>9</v>
+      </c>
+      <c r="R10">
+        <f t="shared" si="4"/>
+        <v>5</v>
+      </c>
       <c r="S10">
-        <f t="shared" si="2"/>
-        <v>17</v>
+        <f t="shared" si="5"/>
+        <v>2</v>
       </c>
       <c r="T10">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <f t="shared" si="6"/>
+        <v>13</v>
       </c>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.25">
@@ -4408,42 +4421,42 @@
       </c>
       <c r="J11">
         <f t="shared" si="0"/>
-        <v>0.68493150700000005</v>
+        <v>0.10159817366666668</v>
       </c>
       <c r="L11">
         <v>9</v>
       </c>
       <c r="M11">
-        <f>M10+M$4</f>
+        <f t="shared" si="8"/>
         <v>0.66666666666666663</v>
       </c>
       <c r="N11">
-        <f>N10+N$3</f>
+        <f t="shared" si="7"/>
         <v>0.75</v>
       </c>
       <c r="O11">
-        <f>COUNTIFS(A:A,"=R. diluvianum",I:I,"&lt;"&amp;N11,I:I,"&gt;="&amp;M11)</f>
-        <v>18</v>
-      </c>
-      <c r="P11">
-        <f>COUNTIFS(A:A,"=A. incurva",I:I,"&lt;"&amp;N11,I:I,"&gt;="&amp;M11)</f>
-        <v>2</v>
-      </c>
-      <c r="Q11">
-        <f>COUNTIFS(A:A,"=B. suecicus",I:I,"&lt;"&amp;N11,I:I,"&gt;="&amp;M11)</f>
-        <v>0</v>
-      </c>
-      <c r="R11">
         <f t="shared" si="1"/>
         <v>18</v>
       </c>
+      <c r="P11">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="Q11">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="R11">
+        <f t="shared" si="4"/>
+        <v>5</v>
+      </c>
       <c r="S11">
-        <f t="shared" si="2"/>
-        <v>28</v>
+        <f t="shared" si="5"/>
+        <v>0</v>
       </c>
       <c r="T11">
-        <f t="shared" si="3"/>
-        <v>4</v>
+        <f t="shared" si="6"/>
+        <v>6</v>
       </c>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.25">
@@ -4476,42 +4489,42 @@
       </c>
       <c r="J12">
         <f t="shared" si="0"/>
-        <v>0.68493150700000005</v>
+        <v>0.10159817366666668</v>
       </c>
       <c r="L12">
         <v>10</v>
       </c>
       <c r="M12">
-        <f>M11+M$4</f>
+        <f t="shared" si="8"/>
         <v>0.75</v>
       </c>
       <c r="N12">
-        <f>N11+N$3</f>
+        <f t="shared" si="7"/>
         <v>0.83333333333333337</v>
       </c>
       <c r="O12">
-        <f>COUNTIFS(A:A,"=R. diluvianum",I:I,"&lt;"&amp;N12,I:I,"&gt;="&amp;M12)</f>
-        <v>10</v>
-      </c>
-      <c r="P12">
-        <f>COUNTIFS(A:A,"=A. incurva",I:I,"&lt;"&amp;N12,I:I,"&gt;="&amp;M12)</f>
-        <v>4</v>
-      </c>
-      <c r="Q12">
-        <f>COUNTIFS(A:A,"=B. suecicus",I:I,"&lt;"&amp;N12,I:I,"&gt;="&amp;M12)</f>
-        <v>4</v>
-      </c>
-      <c r="R12">
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
+      <c r="P12">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="Q12">
+        <f t="shared" si="3"/>
+        <v>4</v>
+      </c>
+      <c r="R12">
+        <f t="shared" si="4"/>
+        <v>6</v>
+      </c>
       <c r="S12">
-        <f t="shared" si="2"/>
-        <v>14</v>
+        <f t="shared" si="5"/>
+        <v>2</v>
       </c>
       <c r="T12">
-        <f t="shared" si="3"/>
-        <v>10</v>
+        <f t="shared" si="6"/>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.25">
@@ -4544,42 +4557,42 @@
       </c>
       <c r="J13">
         <f t="shared" si="0"/>
-        <v>0.68493150700000005</v>
+        <v>0.10159817366666668</v>
       </c>
       <c r="L13">
         <v>11</v>
       </c>
       <c r="M13">
-        <f>M12+M$4</f>
+        <f t="shared" si="8"/>
         <v>0.83333333333333337</v>
       </c>
       <c r="N13">
-        <f>N12+N$3</f>
+        <f t="shared" si="7"/>
         <v>0.91666666666666674</v>
       </c>
       <c r="O13">
-        <f>COUNTIFS(A:A,"=R. diluvianum",I:I,"&lt;"&amp;N13,I:I,"&gt;="&amp;M13)</f>
-        <v>8</v>
-      </c>
-      <c r="P13">
-        <f>COUNTIFS(A:A,"=A. incurva",I:I,"&lt;"&amp;N13,I:I,"&gt;="&amp;M13)</f>
-        <v>0</v>
-      </c>
-      <c r="Q13">
-        <f>COUNTIFS(A:A,"=B. suecicus",I:I,"&lt;"&amp;N13,I:I,"&gt;="&amp;M13)</f>
-        <v>10</v>
-      </c>
-      <c r="R13">
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
-      <c r="S13">
+      <c r="P13">
         <f t="shared" si="2"/>
-        <v>20</v>
-      </c>
-      <c r="T13">
+        <v>0</v>
+      </c>
+      <c r="Q13">
         <f t="shared" si="3"/>
         <v>10</v>
+      </c>
+      <c r="R13">
+        <f t="shared" si="4"/>
+        <v>19</v>
+      </c>
+      <c r="S13">
+        <f t="shared" si="5"/>
+        <v>4</v>
+      </c>
+      <c r="T13">
+        <f t="shared" si="6"/>
+        <v>6</v>
       </c>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.25">
@@ -4612,42 +4625,42 @@
       </c>
       <c r="J14">
         <f t="shared" si="0"/>
-        <v>0.68493150700000005</v>
+        <v>0.10159817366666668</v>
       </c>
       <c r="L14">
         <v>12</v>
       </c>
       <c r="M14">
-        <f>M13+M$4</f>
+        <f t="shared" si="8"/>
         <v>0.91666666666666674</v>
       </c>
       <c r="N14">
-        <f>N13+N$3</f>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="O14">
-        <f>COUNTIFS(A:A,"=R. diluvianum",I:I,"&lt;"&amp;N14,I:I,"&gt;="&amp;M14)</f>
-        <v>4</v>
-      </c>
-      <c r="P14">
-        <f>COUNTIFS(A:A,"=A. incurva",I:I,"&lt;"&amp;N14,I:I,"&gt;="&amp;M14)</f>
-        <v>17</v>
-      </c>
-      <c r="Q14">
-        <f>COUNTIFS(A:A,"=B. suecicus",I:I,"&lt;"&amp;N14,I:I,"&gt;="&amp;M14)</f>
-        <v>10</v>
-      </c>
-      <c r="R14">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
+      <c r="P14">
+        <f t="shared" si="2"/>
+        <v>17</v>
+      </c>
+      <c r="Q14">
+        <f t="shared" si="3"/>
+        <v>10</v>
+      </c>
+      <c r="R14">
+        <f t="shared" si="4"/>
+        <v>16</v>
+      </c>
       <c r="S14">
-        <f t="shared" si="2"/>
-        <v>16</v>
+        <f t="shared" si="5"/>
+        <v>0</v>
       </c>
       <c r="T14">
-        <f t="shared" si="3"/>
-        <v>19</v>
+        <f t="shared" si="6"/>
+        <v>9</v>
       </c>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.25">
@@ -4680,7 +4693,7 @@
       </c>
       <c r="J15">
         <f t="shared" si="0"/>
-        <v>0.41917808200000001</v>
+        <v>0.83584474866666669</v>
       </c>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.25">
@@ -4713,7 +4726,7 @@
       </c>
       <c r="J16">
         <f t="shared" si="0"/>
-        <v>0.41917808200000001</v>
+        <v>0.83584474866666669</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
@@ -4746,7 +4759,7 @@
       </c>
       <c r="J17">
         <f t="shared" si="0"/>
-        <v>0.41917808200000001</v>
+        <v>0.83584474866666669</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
@@ -4779,7 +4792,7 @@
       </c>
       <c r="J18">
         <f t="shared" si="0"/>
-        <v>0.41917808200000001</v>
+        <v>0.83584474866666669</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
@@ -4812,7 +4825,7 @@
       </c>
       <c r="J19">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.41666666666666669</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
@@ -4845,7 +4858,7 @@
       </c>
       <c r="J20">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.41666666666666669</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
@@ -4878,7 +4891,7 @@
       </c>
       <c r="J21">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.41666666666666669</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
@@ -4911,7 +4924,7 @@
       </c>
       <c r="J22">
         <f t="shared" si="0"/>
-        <v>0.90684931499999999</v>
+        <v>0.32351598166666662</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
@@ -4944,7 +4957,7 @@
       </c>
       <c r="J23">
         <f t="shared" si="0"/>
-        <v>0.90684931499999999</v>
+        <v>0.32351598166666662</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
@@ -4977,7 +4990,7 @@
       </c>
       <c r="J24">
         <f t="shared" si="0"/>
-        <v>0.80821917799999998</v>
+        <v>0.22488584466666661</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
@@ -5010,7 +5023,7 @@
       </c>
       <c r="J25">
         <f t="shared" si="0"/>
-        <v>0.68767123299999999</v>
+        <v>0.10433789966666662</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
@@ -5043,7 +5056,7 @@
       </c>
       <c r="J26">
         <f t="shared" si="0"/>
-        <v>0.68767123299999999</v>
+        <v>0.10433789966666662</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
@@ -5076,7 +5089,7 @@
       </c>
       <c r="J27">
         <f t="shared" si="0"/>
-        <v>0.68767123299999999</v>
+        <v>0.10433789966666662</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
@@ -5109,7 +5122,7 @@
       </c>
       <c r="J28">
         <f t="shared" si="0"/>
-        <v>0.68493150700000005</v>
+        <v>0.10159817366666668</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
@@ -5142,7 +5155,7 @@
       </c>
       <c r="J29">
         <f t="shared" si="0"/>
-        <v>0.61369863000000002</v>
+        <v>3.0365296666666763E-2</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
@@ -5175,7 +5188,7 @@
       </c>
       <c r="J30">
         <f t="shared" si="0"/>
-        <v>0.61369863000000002</v>
+        <v>3.0365296666666763E-2</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
@@ -5208,7 +5221,7 @@
       </c>
       <c r="J31">
         <f t="shared" si="0"/>
-        <v>0.61369863000000002</v>
+        <v>3.0365296666666763E-2</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
@@ -5241,7 +5254,7 @@
       </c>
       <c r="J32">
         <f t="shared" si="0"/>
-        <v>0.49041095899999998</v>
+        <v>0.90707762566666661</v>
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
@@ -5274,7 +5287,7 @@
       </c>
       <c r="J33">
         <f t="shared" si="0"/>
-        <v>0.49041095899999998</v>
+        <v>0.90707762566666661</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
@@ -5307,7 +5320,7 @@
       </c>
       <c r="J34">
         <f t="shared" si="0"/>
-        <v>0.36986301399999999</v>
+        <v>0.78652968066666662</v>
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
@@ -5340,7 +5353,7 @@
       </c>
       <c r="J35">
         <f t="shared" si="0"/>
-        <v>0.36986301399999999</v>
+        <v>0.78652968066666662</v>
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
@@ -5373,7 +5386,7 @@
       </c>
       <c r="J36">
         <f t="shared" si="0"/>
-        <v>0.26027397299999999</v>
+        <v>0.67694063966666662</v>
       </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
@@ -5406,7 +5419,7 @@
       </c>
       <c r="J37">
         <f t="shared" si="0"/>
-        <v>0.26027397299999999</v>
+        <v>0.67694063966666662</v>
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
@@ -5439,7 +5452,7 @@
       </c>
       <c r="J38">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.41666666666666669</v>
       </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
@@ -5472,7 +5485,7 @@
       </c>
       <c r="J39">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.41666666666666669</v>
       </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.25">
@@ -5505,7 +5518,7 @@
       </c>
       <c r="J40">
         <f t="shared" si="0"/>
-        <v>7.1232877E-2</v>
+        <v>0.48789954366666666</v>
       </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.25">
@@ -5538,7 +5551,7 @@
       </c>
       <c r="J41">
         <f t="shared" si="0"/>
-        <v>7.1232877E-2</v>
+        <v>0.48789954366666666</v>
       </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.25">
@@ -5571,7 +5584,7 @@
       </c>
       <c r="J42">
         <f t="shared" si="0"/>
-        <v>0.98630136999999996</v>
+        <v>0.40296803666666658</v>
       </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.25">
@@ -5604,7 +5617,7 @@
       </c>
       <c r="J43">
         <f t="shared" si="0"/>
-        <v>0.98630136999999996</v>
+        <v>0.40296803666666658</v>
       </c>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.25">
@@ -5637,7 +5650,7 @@
       </c>
       <c r="J44">
         <f t="shared" si="0"/>
-        <v>0.83287671200000002</v>
+        <v>0.24954337866666676</v>
       </c>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.25">
@@ -5670,7 +5683,7 @@
       </c>
       <c r="J45">
         <f t="shared" si="0"/>
-        <v>0.83287671200000002</v>
+        <v>0.24954337866666676</v>
       </c>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.25">
@@ -5703,7 +5716,7 @@
       </c>
       <c r="J46">
         <f t="shared" si="0"/>
-        <v>0.75890411000000002</v>
+        <v>0.17557077666666676</v>
       </c>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.25">
@@ -5736,7 +5749,7 @@
       </c>
       <c r="J47">
         <f t="shared" si="0"/>
-        <v>0.75890411000000002</v>
+        <v>0.17557077666666676</v>
       </c>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.25">
@@ -5769,7 +5782,7 @@
       </c>
       <c r="J48">
         <f t="shared" si="0"/>
-        <v>0.68767123299999999</v>
+        <v>0.10433789966666662</v>
       </c>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.25">
@@ -5802,7 +5815,7 @@
       </c>
       <c r="J49">
         <f t="shared" si="0"/>
-        <v>0.68767123299999999</v>
+        <v>0.10433789966666662</v>
       </c>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.25">
@@ -5835,7 +5848,7 @@
       </c>
       <c r="J50">
         <f t="shared" si="0"/>
-        <v>0.64109589</v>
+        <v>5.7762556666666631E-2</v>
       </c>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.25">
@@ -5868,7 +5881,7 @@
       </c>
       <c r="J51">
         <f t="shared" si="0"/>
-        <v>0.64109589</v>
+        <v>5.7762556666666631E-2</v>
       </c>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.25">
@@ -5901,7 +5914,7 @@
       </c>
       <c r="J52">
         <f t="shared" si="0"/>
-        <v>0.59452054799999998</v>
+        <v>1.1187214666666723E-2</v>
       </c>
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.25">
@@ -5934,7 +5947,7 @@
       </c>
       <c r="J53">
         <f t="shared" si="0"/>
-        <v>0.59452054799999998</v>
+        <v>1.1187214666666723E-2</v>
       </c>
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.25">
@@ -5967,7 +5980,7 @@
       </c>
       <c r="J54">
         <f t="shared" si="0"/>
-        <v>0.54794520499999999</v>
+        <v>0.96461187166666673</v>
       </c>
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.25">
@@ -6000,7 +6013,7 @@
       </c>
       <c r="J55">
         <f t="shared" si="0"/>
-        <v>0.54794520499999999</v>
+        <v>0.96461187166666673</v>
       </c>
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.25">
@@ -6033,7 +6046,7 @@
       </c>
       <c r="J56">
         <f t="shared" si="0"/>
-        <v>0.50136986299999997</v>
+        <v>0.9180365296666666</v>
       </c>
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.25">
@@ -6066,7 +6079,7 @@
       </c>
       <c r="J57">
         <f t="shared" si="0"/>
-        <v>0.50136986299999997</v>
+        <v>0.9180365296666666</v>
       </c>
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.25">
@@ -6099,7 +6112,7 @@
       </c>
       <c r="J58">
         <f t="shared" si="0"/>
-        <v>0.44931506799999998</v>
+        <v>0.86598173466666672</v>
       </c>
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.25">
@@ -6132,7 +6145,7 @@
       </c>
       <c r="J59">
         <f t="shared" si="0"/>
-        <v>0.44931506799999998</v>
+        <v>0.86598173466666672</v>
       </c>
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.25">
@@ -6165,7 +6178,7 @@
       </c>
       <c r="J60">
         <f t="shared" si="0"/>
-        <v>0.38904109599999998</v>
+        <v>0.80570776266666666</v>
       </c>
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.25">
@@ -6198,7 +6211,7 @@
       </c>
       <c r="J61">
         <f t="shared" si="0"/>
-        <v>0.38904109599999998</v>
+        <v>0.80570776266666666</v>
       </c>
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.25">
@@ -6231,7 +6244,7 @@
       </c>
       <c r="J62">
         <f t="shared" si="0"/>
-        <v>3.2876712000000002E-2</v>
+        <v>0.44954337866666672</v>
       </c>
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.25">
@@ -6264,7 +6277,7 @@
       </c>
       <c r="J63">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.41666666666666669</v>
       </c>
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.25">
@@ -6297,7 +6310,7 @@
       </c>
       <c r="J64">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.41666666666666669</v>
       </c>
     </row>
     <row r="65" spans="1:10" x14ac:dyDescent="0.25">
@@ -6330,7 +6343,7 @@
       </c>
       <c r="J65">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.41666666666666669</v>
       </c>
     </row>
     <row r="66" spans="1:10" x14ac:dyDescent="0.25">
@@ -6363,7 +6376,7 @@
       </c>
       <c r="J66">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.41666666666666669</v>
       </c>
     </row>
     <row r="67" spans="1:10" x14ac:dyDescent="0.25">
@@ -6395,8 +6408,8 @@
         <v>0</v>
       </c>
       <c r="J67">
-        <f t="shared" ref="J67:J130" si="4">IF(A67="R. diluvianum", I67, IF(A67="A. incurva", MOD(I67-4/12, 1), MOD(I67-1/12, 1)))</f>
-        <v>0</v>
+        <f t="shared" ref="J67:J130" si="9">IF(A67="R. diluvianum", MOD(I67+5/12, 1), IF(A67="A. incurva", MOD(I67+1/12, 1), MOD(I67+4/12, 1)))</f>
+        <v>0.41666666666666669</v>
       </c>
     </row>
     <row r="68" spans="1:10" x14ac:dyDescent="0.25">
@@ -6428,8 +6441,8 @@
         <v>0</v>
       </c>
       <c r="J68">
-        <f t="shared" si="4"/>
-        <v>0</v>
+        <f t="shared" si="9"/>
+        <v>0.41666666666666669</v>
       </c>
     </row>
     <row r="69" spans="1:10" x14ac:dyDescent="0.25">
@@ -6461,8 +6474,8 @@
         <v>0</v>
       </c>
       <c r="J69">
-        <f t="shared" si="4"/>
-        <v>0</v>
+        <f t="shared" si="9"/>
+        <v>0.41666666666666669</v>
       </c>
     </row>
     <row r="70" spans="1:10" x14ac:dyDescent="0.25">
@@ -6494,8 +6507,8 @@
         <v>0</v>
       </c>
       <c r="J70">
-        <f t="shared" si="4"/>
-        <v>0</v>
+        <f t="shared" si="9"/>
+        <v>0.41666666666666669</v>
       </c>
     </row>
     <row r="71" spans="1:10" x14ac:dyDescent="0.25">
@@ -6527,8 +6540,8 @@
         <v>0.73698630099999995</v>
       </c>
       <c r="J71">
-        <f t="shared" si="4"/>
-        <v>0.73698630099999995</v>
+        <f t="shared" si="9"/>
+        <v>0.1536529676666667</v>
       </c>
     </row>
     <row r="72" spans="1:10" x14ac:dyDescent="0.25">
@@ -6560,8 +6573,8 @@
         <v>0.73698630099999995</v>
       </c>
       <c r="J72">
-        <f t="shared" si="4"/>
-        <v>0.73698630099999995</v>
+        <f t="shared" si="9"/>
+        <v>0.1536529676666667</v>
       </c>
     </row>
     <row r="73" spans="1:10" x14ac:dyDescent="0.25">
@@ -6593,8 +6606,8 @@
         <v>0.68767123299999999</v>
       </c>
       <c r="J73">
-        <f t="shared" si="4"/>
-        <v>0.68767123299999999</v>
+        <f t="shared" si="9"/>
+        <v>0.10433789966666662</v>
       </c>
     </row>
     <row r="74" spans="1:10" x14ac:dyDescent="0.25">
@@ -6626,8 +6639,8 @@
         <v>0.68767123299999999</v>
       </c>
       <c r="J74">
-        <f t="shared" si="4"/>
-        <v>0.68767123299999999</v>
+        <f t="shared" si="9"/>
+        <v>0.10433789966666662</v>
       </c>
     </row>
     <row r="75" spans="1:10" x14ac:dyDescent="0.25">
@@ -6659,8 +6672,8 @@
         <v>0.62739725999999996</v>
       </c>
       <c r="J75">
-        <f t="shared" si="4"/>
-        <v>0.62739725999999996</v>
+        <f t="shared" si="9"/>
+        <v>4.4063926666666697E-2</v>
       </c>
     </row>
     <row r="76" spans="1:10" x14ac:dyDescent="0.25">
@@ -6692,8 +6705,8 @@
         <v>0.62739725999999996</v>
       </c>
       <c r="J76">
-        <f t="shared" si="4"/>
-        <v>0.62739725999999996</v>
+        <f t="shared" si="9"/>
+        <v>4.4063926666666697E-2</v>
       </c>
     </row>
     <row r="77" spans="1:10" x14ac:dyDescent="0.25">
@@ -6725,8 +6738,8 @@
         <v>0.56438356199999995</v>
       </c>
       <c r="J77">
-        <f t="shared" si="4"/>
-        <v>0.56438356199999995</v>
+        <f t="shared" si="9"/>
+        <v>0.98105022866666669</v>
       </c>
     </row>
     <row r="78" spans="1:10" x14ac:dyDescent="0.25">
@@ -6758,8 +6771,8 @@
         <v>0.56438356199999995</v>
       </c>
       <c r="J78">
-        <f t="shared" si="4"/>
-        <v>0.56438356199999995</v>
+        <f t="shared" si="9"/>
+        <v>0.98105022866666669</v>
       </c>
     </row>
     <row r="79" spans="1:10" x14ac:dyDescent="0.25">
@@ -6791,8 +6804,8 @@
         <v>0.56438356199999995</v>
       </c>
       <c r="J79">
-        <f t="shared" si="4"/>
-        <v>0.56438356199999995</v>
+        <f t="shared" si="9"/>
+        <v>0.98105022866666669</v>
       </c>
     </row>
     <row r="80" spans="1:10" x14ac:dyDescent="0.25">
@@ -6824,8 +6837,8 @@
         <v>0.49589041099999998</v>
       </c>
       <c r="J80">
-        <f t="shared" si="4"/>
-        <v>0.49589041099999998</v>
+        <f t="shared" si="9"/>
+        <v>0.91255707766666672</v>
       </c>
     </row>
     <row r="81" spans="1:10" x14ac:dyDescent="0.25">
@@ -6857,8 +6870,8 @@
         <v>0.49589041099999998</v>
       </c>
       <c r="J81">
-        <f t="shared" si="4"/>
-        <v>0.49589041099999998</v>
+        <f t="shared" si="9"/>
+        <v>0.91255707766666672</v>
       </c>
     </row>
     <row r="82" spans="1:10" x14ac:dyDescent="0.25">
@@ -6890,8 +6903,8 @@
         <v>0.49589041099999998</v>
       </c>
       <c r="J82">
-        <f t="shared" si="4"/>
-        <v>0.49589041099999998</v>
+        <f t="shared" si="9"/>
+        <v>0.91255707766666672</v>
       </c>
     </row>
     <row r="83" spans="1:10" x14ac:dyDescent="0.25">
@@ -6923,8 +6936,8 @@
         <v>0.41643835600000001</v>
       </c>
       <c r="J83">
-        <f t="shared" si="4"/>
-        <v>0.41643835600000001</v>
+        <f t="shared" si="9"/>
+        <v>0.83310502266666675</v>
       </c>
     </row>
     <row r="84" spans="1:10" x14ac:dyDescent="0.25">
@@ -6956,8 +6969,8 @@
         <v>0.41643835600000001</v>
       </c>
       <c r="J84">
-        <f t="shared" si="4"/>
-        <v>0.41643835600000001</v>
+        <f t="shared" si="9"/>
+        <v>0.83310502266666675</v>
       </c>
     </row>
     <row r="85" spans="1:10" x14ac:dyDescent="0.25">
@@ -6989,8 +7002,8 @@
         <v>0.326027397</v>
       </c>
       <c r="J85">
-        <f t="shared" si="4"/>
-        <v>0.326027397</v>
+        <f t="shared" si="9"/>
+        <v>0.74269406366666668</v>
       </c>
     </row>
     <row r="86" spans="1:10" x14ac:dyDescent="0.25">
@@ -7022,8 +7035,8 @@
         <v>0.326027397</v>
       </c>
       <c r="J86">
-        <f t="shared" si="4"/>
-        <v>0.326027397</v>
+        <f t="shared" si="9"/>
+        <v>0.74269406366666668</v>
       </c>
     </row>
     <row r="87" spans="1:10" x14ac:dyDescent="0.25">
@@ -7055,8 +7068,8 @@
         <v>0.208219178</v>
       </c>
       <c r="J87">
-        <f t="shared" si="4"/>
-        <v>0.208219178</v>
+        <f t="shared" si="9"/>
+        <v>0.62488584466666675</v>
       </c>
     </row>
     <row r="88" spans="1:10" x14ac:dyDescent="0.25">
@@ -7088,8 +7101,8 @@
         <v>0.208219178</v>
       </c>
       <c r="J88">
-        <f t="shared" si="4"/>
-        <v>0.208219178</v>
+        <f t="shared" si="9"/>
+        <v>0.62488584466666675</v>
       </c>
     </row>
     <row r="89" spans="1:10" x14ac:dyDescent="0.25">
@@ -7121,8 +7134,8 @@
         <v>0.208219178</v>
       </c>
       <c r="J89">
-        <f t="shared" si="4"/>
-        <v>0.208219178</v>
+        <f t="shared" si="9"/>
+        <v>0.62488584466666675</v>
       </c>
     </row>
     <row r="90" spans="1:10" x14ac:dyDescent="0.25">
@@ -7154,8 +7167,8 @@
         <v>4.6575341999999999E-2</v>
       </c>
       <c r="J90">
-        <f t="shared" si="4"/>
-        <v>4.6575341999999999E-2</v>
+        <f t="shared" si="9"/>
+        <v>0.4632420086666667</v>
       </c>
     </row>
     <row r="91" spans="1:10" x14ac:dyDescent="0.25">
@@ -7187,8 +7200,8 @@
         <v>4.6575341999999999E-2</v>
       </c>
       <c r="J91">
-        <f t="shared" si="4"/>
-        <v>4.6575341999999999E-2</v>
+        <f t="shared" si="9"/>
+        <v>0.4632420086666667</v>
       </c>
     </row>
     <row r="92" spans="1:10" x14ac:dyDescent="0.25">
@@ -7220,8 +7233,8 @@
         <v>0.90410958900000005</v>
       </c>
       <c r="J92">
-        <f t="shared" si="4"/>
-        <v>0.90410958900000005</v>
+        <f t="shared" si="9"/>
+        <v>0.32077625566666668</v>
       </c>
     </row>
     <row r="93" spans="1:10" x14ac:dyDescent="0.25">
@@ -7253,8 +7266,8 @@
         <v>0.90410958900000005</v>
       </c>
       <c r="J93">
-        <f t="shared" si="4"/>
-        <v>0.90410958900000005</v>
+        <f t="shared" si="9"/>
+        <v>0.32077625566666668</v>
       </c>
     </row>
     <row r="94" spans="1:10" x14ac:dyDescent="0.25">
@@ -7286,8 +7299,8 @@
         <v>0.85205479500000003</v>
       </c>
       <c r="J94">
-        <f t="shared" si="4"/>
-        <v>0.85205479500000003</v>
+        <f t="shared" si="9"/>
+        <v>0.26872146166666666</v>
       </c>
     </row>
     <row r="95" spans="1:10" x14ac:dyDescent="0.25">
@@ -7319,8 +7332,8 @@
         <v>0.85205479500000003</v>
       </c>
       <c r="J95">
-        <f t="shared" si="4"/>
-        <v>0.85205479500000003</v>
+        <f t="shared" si="9"/>
+        <v>0.26872146166666666</v>
       </c>
     </row>
     <row r="96" spans="1:10" x14ac:dyDescent="0.25">
@@ -7352,8 +7365,8 @@
         <v>0.8</v>
       </c>
       <c r="J96">
-        <f t="shared" si="4"/>
-        <v>0.8</v>
+        <f t="shared" si="9"/>
+        <v>0.21666666666666679</v>
       </c>
     </row>
     <row r="97" spans="1:10" x14ac:dyDescent="0.25">
@@ -7385,8 +7398,8 @@
         <v>0.8</v>
       </c>
       <c r="J97">
-        <f t="shared" si="4"/>
-        <v>0.8</v>
+        <f t="shared" si="9"/>
+        <v>0.21666666666666679</v>
       </c>
     </row>
     <row r="98" spans="1:10" x14ac:dyDescent="0.25">
@@ -7418,8 +7431,8 @@
         <v>0.745205479</v>
       </c>
       <c r="J98">
-        <f t="shared" si="4"/>
-        <v>0.745205479</v>
+        <f t="shared" si="9"/>
+        <v>0.16187214566666674</v>
       </c>
     </row>
     <row r="99" spans="1:10" x14ac:dyDescent="0.25">
@@ -7451,8 +7464,8 @@
         <v>0.745205479</v>
       </c>
       <c r="J99">
-        <f t="shared" si="4"/>
-        <v>0.745205479</v>
+        <f t="shared" si="9"/>
+        <v>0.16187214566666674</v>
       </c>
     </row>
     <row r="100" spans="1:10" x14ac:dyDescent="0.25">
@@ -7484,8 +7497,8 @@
         <v>0.68767123299999999</v>
       </c>
       <c r="J100">
-        <f t="shared" si="4"/>
-        <v>0.68767123299999999</v>
+        <f t="shared" si="9"/>
+        <v>0.10433789966666662</v>
       </c>
     </row>
     <row r="101" spans="1:10" x14ac:dyDescent="0.25">
@@ -7517,8 +7530,8 @@
         <v>0.68767123299999999</v>
       </c>
       <c r="J101">
-        <f t="shared" si="4"/>
-        <v>0.68767123299999999</v>
+        <f t="shared" si="9"/>
+        <v>0.10433789966666662</v>
       </c>
     </row>
     <row r="102" spans="1:10" x14ac:dyDescent="0.25">
@@ -7550,8 +7563,8 @@
         <v>0.63013698600000001</v>
       </c>
       <c r="J102">
-        <f t="shared" si="4"/>
-        <v>0.63013698600000001</v>
+        <f t="shared" si="9"/>
+        <v>4.680365266666664E-2</v>
       </c>
     </row>
     <row r="103" spans="1:10" x14ac:dyDescent="0.25">
@@ -7583,8 +7596,8 @@
         <v>0.63013698600000001</v>
       </c>
       <c r="J103">
-        <f t="shared" si="4"/>
-        <v>0.63013698600000001</v>
+        <f t="shared" si="9"/>
+        <v>4.680365266666664E-2</v>
       </c>
     </row>
     <row r="104" spans="1:10" x14ac:dyDescent="0.25">
@@ -7616,8 +7629,8 @@
         <v>0.63013698600000001</v>
       </c>
       <c r="J104">
-        <f t="shared" si="4"/>
-        <v>0.63013698600000001</v>
+        <f t="shared" si="9"/>
+        <v>4.680365266666664E-2</v>
       </c>
     </row>
     <row r="105" spans="1:10" x14ac:dyDescent="0.25">
@@ -7649,8 +7662,8 @@
         <v>0.567123288</v>
       </c>
       <c r="J105">
-        <f t="shared" si="4"/>
-        <v>0.567123288</v>
+        <f t="shared" si="9"/>
+        <v>0.98378995466666663</v>
       </c>
     </row>
     <row r="106" spans="1:10" x14ac:dyDescent="0.25">
@@ -7682,8 +7695,8 @@
         <v>0.567123288</v>
       </c>
       <c r="J106">
-        <f t="shared" si="4"/>
-        <v>0.567123288</v>
+        <f t="shared" si="9"/>
+        <v>0.98378995466666663</v>
       </c>
     </row>
     <row r="107" spans="1:10" x14ac:dyDescent="0.25">
@@ -7715,8 +7728,8 @@
         <v>0.567123288</v>
       </c>
       <c r="J107">
-        <f t="shared" si="4"/>
-        <v>0.567123288</v>
+        <f t="shared" si="9"/>
+        <v>0.98378995466666663</v>
       </c>
     </row>
     <row r="108" spans="1:10" x14ac:dyDescent="0.25">
@@ -7748,8 +7761,8 @@
         <v>0.567123288</v>
       </c>
       <c r="J108">
-        <f t="shared" si="4"/>
-        <v>0.567123288</v>
+        <f t="shared" si="9"/>
+        <v>0.98378995466666663</v>
       </c>
     </row>
     <row r="109" spans="1:10" x14ac:dyDescent="0.25">
@@ -7781,8 +7794,8 @@
         <v>0.567123288</v>
       </c>
       <c r="J109">
-        <f t="shared" si="4"/>
-        <v>0.567123288</v>
+        <f t="shared" si="9"/>
+        <v>0.98378995466666663</v>
       </c>
     </row>
     <row r="110" spans="1:10" x14ac:dyDescent="0.25">
@@ -7814,8 +7827,8 @@
         <v>0.567123288</v>
       </c>
       <c r="J110">
-        <f t="shared" si="4"/>
-        <v>0.567123288</v>
+        <f t="shared" si="9"/>
+        <v>0.98378995466666663</v>
       </c>
     </row>
     <row r="111" spans="1:10" x14ac:dyDescent="0.25">
@@ -7847,8 +7860,8 @@
         <v>0.567123288</v>
       </c>
       <c r="J111">
-        <f t="shared" si="4"/>
-        <v>0.567123288</v>
+        <f t="shared" si="9"/>
+        <v>0.98378995466666663</v>
       </c>
     </row>
     <row r="112" spans="1:10" x14ac:dyDescent="0.25">
@@ -7880,8 +7893,8 @@
         <v>0.567123288</v>
       </c>
       <c r="J112">
-        <f t="shared" si="4"/>
-        <v>0.567123288</v>
+        <f t="shared" si="9"/>
+        <v>0.98378995466666663</v>
       </c>
     </row>
     <row r="113" spans="1:10" x14ac:dyDescent="0.25">
@@ -7913,8 +7926,8 @@
         <v>0.567123288</v>
       </c>
       <c r="J113">
-        <f t="shared" si="4"/>
-        <v>0.567123288</v>
+        <f t="shared" si="9"/>
+        <v>0.98378995466666663</v>
       </c>
     </row>
     <row r="114" spans="1:10" x14ac:dyDescent="0.25">
@@ -7946,8 +7959,8 @@
         <v>0.49863013699999997</v>
       </c>
       <c r="J114">
-        <f t="shared" si="4"/>
-        <v>0.49863013699999997</v>
+        <f t="shared" si="9"/>
+        <v>0.91529680366666666</v>
       </c>
     </row>
     <row r="115" spans="1:10" x14ac:dyDescent="0.25">
@@ -7979,8 +7992,8 @@
         <v>0.49863013699999997</v>
       </c>
       <c r="J115">
-        <f t="shared" si="4"/>
-        <v>0.49863013699999997</v>
+        <f t="shared" si="9"/>
+        <v>0.91529680366666666</v>
       </c>
     </row>
     <row r="116" spans="1:10" x14ac:dyDescent="0.25">
@@ -8012,8 +8025,8 @@
         <v>0.42191780800000001</v>
       </c>
       <c r="J116">
-        <f t="shared" si="4"/>
-        <v>0.42191780800000001</v>
+        <f t="shared" si="9"/>
+        <v>0.83858447466666663</v>
       </c>
     </row>
     <row r="117" spans="1:10" x14ac:dyDescent="0.25">
@@ -8045,8 +8058,8 @@
         <v>0.42191780800000001</v>
       </c>
       <c r="J117">
-        <f t="shared" si="4"/>
-        <v>0.42191780800000001</v>
+        <f t="shared" si="9"/>
+        <v>0.83858447466666663</v>
       </c>
     </row>
     <row r="118" spans="1:10" x14ac:dyDescent="0.25">
@@ -8078,8 +8091,8 @@
         <v>0.42191780800000001</v>
       </c>
       <c r="J118">
-        <f t="shared" si="4"/>
-        <v>0.42191780800000001</v>
+        <f t="shared" si="9"/>
+        <v>0.83858447466666663</v>
       </c>
     </row>
     <row r="119" spans="1:10" x14ac:dyDescent="0.25">
@@ -8111,8 +8124,8 @@
         <v>0.42191780800000001</v>
       </c>
       <c r="J119">
-        <f t="shared" si="4"/>
-        <v>0.42191780800000001</v>
+        <f t="shared" si="9"/>
+        <v>0.83858447466666663</v>
       </c>
     </row>
     <row r="120" spans="1:10" x14ac:dyDescent="0.25">
@@ -8144,8 +8157,8 @@
         <v>0.42191780800000001</v>
       </c>
       <c r="J120">
-        <f t="shared" si="4"/>
-        <v>0.42191780800000001</v>
+        <f t="shared" si="9"/>
+        <v>0.83858447466666663</v>
       </c>
     </row>
     <row r="121" spans="1:10" x14ac:dyDescent="0.25">
@@ -8177,8 +8190,8 @@
         <v>0.42191780800000001</v>
       </c>
       <c r="J121">
-        <f t="shared" si="4"/>
-        <v>0.42191780800000001</v>
+        <f t="shared" si="9"/>
+        <v>0.83858447466666663</v>
       </c>
     </row>
     <row r="122" spans="1:10" x14ac:dyDescent="0.25">
@@ -8210,8 +8223,8 @@
         <v>0.32876712299999999</v>
       </c>
       <c r="J122">
-        <f t="shared" si="4"/>
-        <v>0.32876712299999999</v>
+        <f t="shared" si="9"/>
+        <v>0.74543378966666674</v>
       </c>
     </row>
     <row r="123" spans="1:10" x14ac:dyDescent="0.25">
@@ -8243,8 +8256,8 @@
         <v>0.142465753</v>
       </c>
       <c r="J123">
-        <f t="shared" si="4"/>
-        <v>0.80913241966666671</v>
+        <f t="shared" si="9"/>
+        <v>0.22579908633333334</v>
       </c>
     </row>
     <row r="124" spans="1:10" x14ac:dyDescent="0.25">
@@ -8276,8 +8289,8 @@
         <v>0.142465753</v>
       </c>
       <c r="J124">
-        <f t="shared" si="4"/>
-        <v>0.80913241966666671</v>
+        <f t="shared" si="9"/>
+        <v>0.22579908633333334</v>
       </c>
     </row>
     <row r="125" spans="1:10" x14ac:dyDescent="0.25">
@@ -8309,8 +8322,8 @@
         <v>0.20273972600000001</v>
       </c>
       <c r="J125">
-        <f t="shared" si="4"/>
-        <v>0.86940639266666664</v>
+        <f t="shared" si="9"/>
+        <v>0.28607305933333332</v>
       </c>
     </row>
     <row r="126" spans="1:10" x14ac:dyDescent="0.25">
@@ -8342,8 +8355,8 @@
         <v>0.25753424699999999</v>
       </c>
       <c r="J126">
-        <f t="shared" si="4"/>
-        <v>0.92420091366666668</v>
+        <f t="shared" si="9"/>
+        <v>0.34086758033333331</v>
       </c>
     </row>
     <row r="127" spans="1:10" x14ac:dyDescent="0.25">
@@ -8375,8 +8388,8 @@
         <v>0.25753424699999999</v>
       </c>
       <c r="J127">
-        <f t="shared" si="4"/>
-        <v>0.92420091366666668</v>
+        <f t="shared" si="9"/>
+        <v>0.34086758033333331</v>
       </c>
     </row>
     <row r="128" spans="1:10" x14ac:dyDescent="0.25">
@@ -8408,8 +8421,8 @@
         <v>0.31232876700000001</v>
       </c>
       <c r="J128">
-        <f t="shared" si="4"/>
-        <v>0.97899543366666664</v>
+        <f t="shared" si="9"/>
+        <v>0.39566210033333332</v>
       </c>
     </row>
     <row r="129" spans="1:10" x14ac:dyDescent="0.25">
@@ -8441,8 +8454,8 @@
         <v>0.36438356199999999</v>
       </c>
       <c r="J129">
-        <f t="shared" si="4"/>
-        <v>3.1050228666666679E-2</v>
+        <f t="shared" si="9"/>
+        <v>0.44771689533333331</v>
       </c>
     </row>
     <row r="130" spans="1:10" x14ac:dyDescent="0.25">
@@ -8474,8 +8487,8 @@
         <v>0.36438356199999999</v>
       </c>
       <c r="J130">
-        <f t="shared" si="4"/>
-        <v>3.1050228666666679E-2</v>
+        <f t="shared" si="9"/>
+        <v>0.44771689533333331</v>
       </c>
     </row>
     <row r="131" spans="1:10" x14ac:dyDescent="0.25">
@@ -8507,8 +8520,8 @@
         <v>0.36438356199999999</v>
       </c>
       <c r="J131">
-        <f t="shared" ref="J131:J194" si="5">IF(A131="R. diluvianum", I131, IF(A131="A. incurva", MOD(I131-4/12, 1), MOD(I131-1/12, 1)))</f>
-        <v>3.1050228666666679E-2</v>
+        <f t="shared" ref="J131:J194" si="10">IF(A131="R. diluvianum", MOD(I131+5/12, 1), IF(A131="A. incurva", MOD(I131+1/12, 1), MOD(I131+4/12, 1)))</f>
+        <v>0.44771689533333331</v>
       </c>
     </row>
     <row r="132" spans="1:10" x14ac:dyDescent="0.25">
@@ -8540,8 +8553,8 @@
         <v>0.83013698599999997</v>
       </c>
       <c r="J132">
-        <f t="shared" si="5"/>
-        <v>0.49680365266666665</v>
+        <f t="shared" si="10"/>
+        <v>0.91347031933333334</v>
       </c>
     </row>
     <row r="133" spans="1:10" x14ac:dyDescent="0.25">
@@ -8573,8 +8586,8 @@
         <v>0.83013698599999997</v>
       </c>
       <c r="J133">
-        <f t="shared" si="5"/>
-        <v>0.49680365266666665</v>
+        <f t="shared" si="10"/>
+        <v>0.91347031933333334</v>
       </c>
     </row>
     <row r="134" spans="1:10" x14ac:dyDescent="0.25">
@@ -8606,8 +8619,8 @@
         <v>0.83013698599999997</v>
       </c>
       <c r="J134">
-        <f t="shared" si="5"/>
-        <v>0.49680365266666665</v>
+        <f t="shared" si="10"/>
+        <v>0.91347031933333334</v>
       </c>
     </row>
     <row r="135" spans="1:10" x14ac:dyDescent="0.25">
@@ -8639,8 +8652,8 @@
         <v>0.83013698599999997</v>
       </c>
       <c r="J135">
-        <f t="shared" si="5"/>
-        <v>0.49680365266666665</v>
+        <f t="shared" si="10"/>
+        <v>0.91347031933333334</v>
       </c>
     </row>
     <row r="136" spans="1:10" x14ac:dyDescent="0.25">
@@ -8672,8 +8685,8 @@
         <v>0.95890410999999998</v>
       </c>
       <c r="J136">
-        <f t="shared" si="5"/>
-        <v>0.62557077666666672</v>
+        <f t="shared" si="10"/>
+        <v>4.2237443333333236E-2</v>
       </c>
     </row>
     <row r="137" spans="1:10" x14ac:dyDescent="0.25">
@@ -8705,8 +8718,8 @@
         <v>0.95890410999999998</v>
       </c>
       <c r="J137">
-        <f t="shared" si="5"/>
-        <v>0.62557077666666672</v>
+        <f t="shared" si="10"/>
+        <v>4.2237443333333236E-2</v>
       </c>
     </row>
     <row r="138" spans="1:10" x14ac:dyDescent="0.25">
@@ -8738,8 +8751,8 @@
         <v>4.6575341999999999E-2</v>
       </c>
       <c r="J138">
-        <f t="shared" si="5"/>
-        <v>0.71324200866666665</v>
+        <f t="shared" si="10"/>
+        <v>0.12990867533333333</v>
       </c>
     </row>
     <row r="139" spans="1:10" x14ac:dyDescent="0.25">
@@ -8771,8 +8784,8 @@
         <v>4.6575341999999999E-2</v>
       </c>
       <c r="J139">
-        <f t="shared" si="5"/>
-        <v>0.71324200866666665</v>
+        <f t="shared" si="10"/>
+        <v>0.12990867533333333</v>
       </c>
     </row>
     <row r="140" spans="1:10" x14ac:dyDescent="0.25">
@@ -8804,8 +8817,8 @@
         <v>4.6575341999999999E-2</v>
       </c>
       <c r="J140">
-        <f t="shared" si="5"/>
-        <v>0.71324200866666665</v>
+        <f t="shared" si="10"/>
+        <v>0.12990867533333333</v>
       </c>
     </row>
     <row r="141" spans="1:10" x14ac:dyDescent="0.25">
@@ -8837,8 +8850,8 @@
         <v>4.6575341999999999E-2</v>
       </c>
       <c r="J141">
-        <f t="shared" si="5"/>
-        <v>0.71324200866666665</v>
+        <f t="shared" si="10"/>
+        <v>0.12990867533333333</v>
       </c>
     </row>
     <row r="142" spans="1:10" x14ac:dyDescent="0.25">
@@ -8870,8 +8883,8 @@
         <v>0.11506849299999999</v>
       </c>
       <c r="J142">
-        <f t="shared" si="5"/>
-        <v>0.78173515966666662</v>
+        <f t="shared" si="10"/>
+        <v>0.19840182633333331</v>
       </c>
     </row>
     <row r="143" spans="1:10" x14ac:dyDescent="0.25">
@@ -8903,8 +8916,8 @@
         <v>0.11506849299999999</v>
       </c>
       <c r="J143">
-        <f t="shared" si="5"/>
-        <v>0.78173515966666662</v>
+        <f t="shared" si="10"/>
+        <v>0.19840182633333331</v>
       </c>
     </row>
     <row r="144" spans="1:10" x14ac:dyDescent="0.25">
@@ -8936,8 +8949,8 @@
         <v>0.178082192</v>
       </c>
       <c r="J144">
-        <f t="shared" si="5"/>
-        <v>0.84474885866666671</v>
+        <f t="shared" si="10"/>
+        <v>0.26141552533333334</v>
       </c>
     </row>
     <row r="145" spans="1:10" x14ac:dyDescent="0.25">
@@ -8969,8 +8982,8 @@
         <v>0.178082192</v>
       </c>
       <c r="J145">
-        <f t="shared" si="5"/>
-        <v>0.84474885866666671</v>
+        <f t="shared" si="10"/>
+        <v>0.26141552533333334</v>
       </c>
     </row>
     <row r="146" spans="1:10" x14ac:dyDescent="0.25">
@@ -9002,8 +9015,8 @@
         <v>0.178082192</v>
       </c>
       <c r="J146">
-        <f t="shared" si="5"/>
-        <v>0.84474885866666671</v>
+        <f t="shared" si="10"/>
+        <v>0.26141552533333334</v>
       </c>
     </row>
     <row r="147" spans="1:10" x14ac:dyDescent="0.25">
@@ -9035,8 +9048,8 @@
         <v>0.23561643800000001</v>
       </c>
       <c r="J147">
-        <f t="shared" si="5"/>
-        <v>0.90228310466666672</v>
+        <f t="shared" si="10"/>
+        <v>0.31894977133333335</v>
       </c>
     </row>
     <row r="148" spans="1:10" x14ac:dyDescent="0.25">
@@ -9068,8 +9081,8 @@
         <v>0.29041095900000002</v>
       </c>
       <c r="J148">
-        <f t="shared" si="5"/>
-        <v>0.95707762566666665</v>
+        <f t="shared" si="10"/>
+        <v>0.37374429233333334</v>
       </c>
     </row>
     <row r="149" spans="1:10" x14ac:dyDescent="0.25">
@@ -9101,8 +9114,8 @@
         <v>0.29041095900000002</v>
       </c>
       <c r="J149">
-        <f t="shared" si="5"/>
-        <v>0.95707762566666665</v>
+        <f t="shared" si="10"/>
+        <v>0.37374429233333334</v>
       </c>
     </row>
     <row r="150" spans="1:10" x14ac:dyDescent="0.25">
@@ -9134,8 +9147,8 @@
         <v>0.34246575299999998</v>
       </c>
       <c r="J150">
-        <f t="shared" si="5"/>
-        <v>9.132419666666669E-3</v>
+        <f t="shared" si="10"/>
+        <v>0.4257990863333333</v>
       </c>
     </row>
     <row r="151" spans="1:10" x14ac:dyDescent="0.25">
@@ -9167,8 +9180,8 @@
         <v>0.34246575299999998</v>
       </c>
       <c r="J151">
-        <f t="shared" si="5"/>
-        <v>9.132419666666669E-3</v>
+        <f t="shared" si="10"/>
+        <v>0.4257990863333333</v>
       </c>
     </row>
     <row r="152" spans="1:10" x14ac:dyDescent="0.25">
@@ -9200,8 +9213,8 @@
         <v>0.93698630100000002</v>
       </c>
       <c r="J152">
-        <f t="shared" si="5"/>
-        <v>0.60365296766666665</v>
+        <f t="shared" si="10"/>
+        <v>2.0319634333333392E-2</v>
       </c>
     </row>
     <row r="153" spans="1:10" x14ac:dyDescent="0.25">
@@ -9233,8 +9246,8 @@
         <v>0.93698630100000002</v>
       </c>
       <c r="J153">
-        <f t="shared" si="5"/>
-        <v>0.60365296766666665</v>
+        <f t="shared" si="10"/>
+        <v>2.0319634333333392E-2</v>
       </c>
     </row>
     <row r="154" spans="1:10" x14ac:dyDescent="0.25">
@@ -9266,8 +9279,8 @@
         <v>0.93698630100000002</v>
       </c>
       <c r="J154">
-        <f t="shared" si="5"/>
-        <v>0.60365296766666665</v>
+        <f t="shared" si="10"/>
+        <v>2.0319634333333392E-2</v>
       </c>
     </row>
     <row r="155" spans="1:10" x14ac:dyDescent="0.25">
@@ -9299,8 +9312,8 @@
         <v>0.96986301399999997</v>
       </c>
       <c r="J155">
-        <f t="shared" si="5"/>
-        <v>0.63652968066666671</v>
+        <f t="shared" si="10"/>
+        <v>5.3196347333333227E-2</v>
       </c>
     </row>
     <row r="156" spans="1:10" x14ac:dyDescent="0.25">
@@ -9332,8 +9345,8 @@
         <v>0.96986301399999997</v>
       </c>
       <c r="J156">
-        <f t="shared" si="5"/>
-        <v>0.63652968066666671</v>
+        <f t="shared" si="10"/>
+        <v>5.3196347333333227E-2</v>
       </c>
     </row>
     <row r="157" spans="1:10" x14ac:dyDescent="0.25">
@@ -9365,8 +9378,8 @@
         <v>2.7397260000000001E-3</v>
       </c>
       <c r="J157">
-        <f t="shared" si="5"/>
-        <v>0.66940639266666668</v>
+        <f t="shared" si="10"/>
+        <v>8.6073059333333327E-2</v>
       </c>
     </row>
     <row r="158" spans="1:10" x14ac:dyDescent="0.25">
@@ -9398,8 +9411,8 @@
         <v>2.7397260000000001E-3</v>
       </c>
       <c r="J158">
-        <f t="shared" si="5"/>
-        <v>0.66940639266666668</v>
+        <f t="shared" si="10"/>
+        <v>8.6073059333333327E-2</v>
       </c>
     </row>
     <row r="159" spans="1:10" x14ac:dyDescent="0.25">
@@ -9431,8 +9444,8 @@
         <v>2.7397260000000001E-3</v>
       </c>
       <c r="J159">
-        <f t="shared" si="5"/>
-        <v>0.66940639266666668</v>
+        <f t="shared" si="10"/>
+        <v>8.6073059333333327E-2</v>
       </c>
     </row>
     <row r="160" spans="1:10" x14ac:dyDescent="0.25">
@@ -9464,8 +9477,8 @@
         <v>3.2876712000000002E-2</v>
       </c>
       <c r="J160">
-        <f t="shared" si="5"/>
-        <v>0.69954337866666672</v>
+        <f t="shared" si="10"/>
+        <v>0.11621004533333333</v>
       </c>
     </row>
     <row r="161" spans="1:10" x14ac:dyDescent="0.25">
@@ -9497,8 +9510,8 @@
         <v>6.5753425000000004E-2</v>
       </c>
       <c r="J161">
-        <f t="shared" si="5"/>
-        <v>0.73242009166666666</v>
+        <f t="shared" si="10"/>
+        <v>0.14908675833333335</v>
       </c>
     </row>
     <row r="162" spans="1:10" x14ac:dyDescent="0.25">
@@ -9530,8 +9543,8 @@
         <v>6.5753425000000004E-2</v>
       </c>
       <c r="J162">
-        <f t="shared" si="5"/>
-        <v>0.73242009166666666</v>
+        <f t="shared" si="10"/>
+        <v>0.14908675833333335</v>
       </c>
     </row>
     <row r="163" spans="1:10" x14ac:dyDescent="0.25">
@@ -9563,8 +9576,8 @@
         <v>6.5753425000000004E-2</v>
       </c>
       <c r="J163">
-        <f t="shared" si="5"/>
-        <v>0.73242009166666666</v>
+        <f t="shared" si="10"/>
+        <v>0.14908675833333335</v>
       </c>
     </row>
     <row r="164" spans="1:10" x14ac:dyDescent="0.25">
@@ -9596,8 +9609,8 @@
         <v>9.8630137000000007E-2</v>
       </c>
       <c r="J164">
-        <f t="shared" si="5"/>
-        <v>0.76529680366666675</v>
+        <f t="shared" si="10"/>
+        <v>0.18196347033333332</v>
       </c>
     </row>
     <row r="165" spans="1:10" x14ac:dyDescent="0.25">
@@ -9629,8 +9642,8 @@
         <v>9.8630137000000007E-2</v>
       </c>
       <c r="J165">
-        <f t="shared" si="5"/>
-        <v>0.76529680366666675</v>
+        <f t="shared" si="10"/>
+        <v>0.18196347033333332</v>
       </c>
     </row>
     <row r="166" spans="1:10" x14ac:dyDescent="0.25">
@@ -9662,8 +9675,8 @@
         <v>0.13424657500000001</v>
       </c>
       <c r="J166">
-        <f t="shared" si="5"/>
-        <v>0.80091324166666666</v>
+        <f t="shared" si="10"/>
+        <v>0.21757990833333335</v>
       </c>
     </row>
     <row r="167" spans="1:10" x14ac:dyDescent="0.25">
@@ -9695,8 +9708,8 @@
         <v>0.13424657500000001</v>
       </c>
       <c r="J167">
-        <f t="shared" si="5"/>
-        <v>0.80091324166666666</v>
+        <f t="shared" si="10"/>
+        <v>0.21757990833333335</v>
       </c>
     </row>
     <row r="168" spans="1:10" x14ac:dyDescent="0.25">
@@ -9728,8 +9741,8 @@
         <v>0.16986301400000001</v>
       </c>
       <c r="J168">
-        <f t="shared" si="5"/>
-        <v>0.83652968066666666</v>
+        <f t="shared" si="10"/>
+        <v>0.25319634733333335</v>
       </c>
     </row>
     <row r="169" spans="1:10" x14ac:dyDescent="0.25">
@@ -9761,8 +9774,8 @@
         <v>0.16986301400000001</v>
       </c>
       <c r="J169">
-        <f t="shared" si="5"/>
-        <v>0.83652968066666666</v>
+        <f t="shared" si="10"/>
+        <v>0.25319634733333335</v>
       </c>
     </row>
     <row r="170" spans="1:10" x14ac:dyDescent="0.25">
@@ -9794,8 +9807,8 @@
         <v>0.16986301400000001</v>
       </c>
       <c r="J170">
-        <f t="shared" si="5"/>
-        <v>0.83652968066666666</v>
+        <f t="shared" si="10"/>
+        <v>0.25319634733333335</v>
       </c>
     </row>
     <row r="171" spans="1:10" x14ac:dyDescent="0.25">
@@ -9827,8 +9840,8 @@
         <v>0.208219178</v>
       </c>
       <c r="J171">
-        <f t="shared" si="5"/>
-        <v>0.87488584466666675</v>
+        <f t="shared" si="10"/>
+        <v>0.29155251133333332</v>
       </c>
     </row>
     <row r="172" spans="1:10" x14ac:dyDescent="0.25">
@@ -9860,8 +9873,8 @@
         <v>0.208219178</v>
       </c>
       <c r="J172">
-        <f t="shared" si="5"/>
-        <v>0.87488584466666675</v>
+        <f t="shared" si="10"/>
+        <v>0.29155251133333332</v>
       </c>
     </row>
     <row r="173" spans="1:10" x14ac:dyDescent="0.25">
@@ -9893,8 +9906,8 @@
         <v>0.208219178</v>
       </c>
       <c r="J173">
-        <f t="shared" si="5"/>
-        <v>0.87488584466666675</v>
+        <f t="shared" si="10"/>
+        <v>0.29155251133333332</v>
       </c>
     </row>
     <row r="174" spans="1:10" x14ac:dyDescent="0.25">
@@ -9926,8 +9939,8 @@
         <v>0.208219178</v>
       </c>
       <c r="J174">
-        <f t="shared" si="5"/>
-        <v>0.87488584466666675</v>
+        <f t="shared" si="10"/>
+        <v>0.29155251133333332</v>
       </c>
     </row>
     <row r="175" spans="1:10" x14ac:dyDescent="0.25">
@@ -9959,8 +9972,8 @@
         <v>0.249315068</v>
       </c>
       <c r="J175">
-        <f t="shared" si="5"/>
-        <v>0.91598173466666666</v>
+        <f t="shared" si="10"/>
+        <v>0.33264840133333334</v>
       </c>
     </row>
     <row r="176" spans="1:10" x14ac:dyDescent="0.25">
@@ -9992,8 +10005,8 @@
         <v>0.249315068</v>
       </c>
       <c r="J176">
-        <f t="shared" si="5"/>
-        <v>0.91598173466666666</v>
+        <f t="shared" si="10"/>
+        <v>0.33264840133333334</v>
       </c>
     </row>
     <row r="177" spans="1:10" x14ac:dyDescent="0.25">
@@ -10025,8 +10038,8 @@
         <v>0.29589041100000002</v>
       </c>
       <c r="J177">
-        <f t="shared" si="5"/>
-        <v>0.96255707766666676</v>
+        <f t="shared" si="10"/>
+        <v>0.37922374433333333</v>
       </c>
     </row>
     <row r="178" spans="1:10" x14ac:dyDescent="0.25">
@@ -10058,8 +10071,8 @@
         <v>0.29589041100000002</v>
       </c>
       <c r="J178">
-        <f t="shared" si="5"/>
-        <v>0.96255707766666676</v>
+        <f t="shared" si="10"/>
+        <v>0.37922374433333333</v>
       </c>
     </row>
     <row r="179" spans="1:10" x14ac:dyDescent="0.25">
@@ -10091,8 +10104,8 @@
         <v>0.350684932</v>
       </c>
       <c r="J179">
-        <f t="shared" si="5"/>
-        <v>1.735159866666669E-2</v>
+        <f t="shared" si="10"/>
+        <v>0.43401826533333332</v>
       </c>
     </row>
     <row r="180" spans="1:10" x14ac:dyDescent="0.25">
@@ -10124,8 +10137,8 @@
         <v>0.350684932</v>
       </c>
       <c r="J180">
-        <f t="shared" si="5"/>
-        <v>1.735159866666669E-2</v>
+        <f t="shared" si="10"/>
+        <v>0.43401826533333332</v>
       </c>
     </row>
     <row r="181" spans="1:10" x14ac:dyDescent="0.25">
@@ -10157,8 +10170,8 @@
         <v>0.424657534</v>
       </c>
       <c r="J181">
-        <f t="shared" si="5"/>
-        <v>9.1324200666666688E-2</v>
+        <f t="shared" si="10"/>
+        <v>0.50799086733333332</v>
       </c>
     </row>
     <row r="182" spans="1:10" x14ac:dyDescent="0.25">
@@ -10190,8 +10203,8 @@
         <v>0.93424657499999997</v>
       </c>
       <c r="J182">
-        <f t="shared" si="5"/>
-        <v>0.60091324166666671</v>
+        <f t="shared" si="10"/>
+        <v>1.7579908333333227E-2</v>
       </c>
     </row>
     <row r="183" spans="1:10" x14ac:dyDescent="0.25">
@@ -10223,8 +10236,8 @@
         <v>0.93424657499999997</v>
       </c>
       <c r="J183">
-        <f t="shared" si="5"/>
-        <v>0.60091324166666671</v>
+        <f t="shared" si="10"/>
+        <v>1.7579908333333227E-2</v>
       </c>
     </row>
     <row r="184" spans="1:10" x14ac:dyDescent="0.25">
@@ -10256,8 +10269,8 @@
         <v>0.96712328800000003</v>
       </c>
       <c r="J184">
-        <f t="shared" si="5"/>
-        <v>0.63378995466666677</v>
+        <f t="shared" si="10"/>
+        <v>5.0456621333333285E-2</v>
       </c>
     </row>
     <row r="185" spans="1:10" x14ac:dyDescent="0.25">
@@ -10289,8 +10302,8 @@
         <v>0.96712328800000003</v>
       </c>
       <c r="J185">
-        <f t="shared" si="5"/>
-        <v>0.63378995466666677</v>
+        <f t="shared" si="10"/>
+        <v>5.0456621333333285E-2</v>
       </c>
     </row>
     <row r="186" spans="1:10" x14ac:dyDescent="0.25">
@@ -10322,8 +10335,8 @@
         <v>0</v>
       </c>
       <c r="J186">
-        <f t="shared" si="5"/>
-        <v>0.66666666666666674</v>
+        <f t="shared" si="10"/>
+        <v>8.3333333333333329E-2</v>
       </c>
     </row>
     <row r="187" spans="1:10" x14ac:dyDescent="0.25">
@@ -10355,8 +10368,8 @@
         <v>0</v>
       </c>
       <c r="J187">
-        <f t="shared" si="5"/>
-        <v>0.66666666666666674</v>
+        <f t="shared" si="10"/>
+        <v>8.3333333333333329E-2</v>
       </c>
     </row>
     <row r="188" spans="1:10" x14ac:dyDescent="0.25">
@@ -10388,8 +10401,8 @@
         <v>3.0136986000000001E-2</v>
       </c>
       <c r="J188">
-        <f t="shared" si="5"/>
-        <v>0.69680365266666666</v>
+        <f t="shared" si="10"/>
+        <v>0.11347031933333333</v>
       </c>
     </row>
     <row r="189" spans="1:10" x14ac:dyDescent="0.25">
@@ -10421,8 +10434,8 @@
         <v>3.0136986000000001E-2</v>
       </c>
       <c r="J189">
-        <f t="shared" si="5"/>
-        <v>0.69680365266666666</v>
+        <f t="shared" si="10"/>
+        <v>0.11347031933333333</v>
       </c>
     </row>
     <row r="190" spans="1:10" x14ac:dyDescent="0.25">
@@ -10454,8 +10467,8 @@
         <v>6.3013699000000006E-2</v>
       </c>
       <c r="J190">
-        <f t="shared" si="5"/>
-        <v>0.72968036566666672</v>
+        <f t="shared" si="10"/>
+        <v>0.14634703233333335</v>
       </c>
     </row>
     <row r="191" spans="1:10" x14ac:dyDescent="0.25">
@@ -10487,8 +10500,8 @@
         <v>6.3013699000000006E-2</v>
       </c>
       <c r="J191">
-        <f t="shared" si="5"/>
-        <v>0.72968036566666672</v>
+        <f t="shared" si="10"/>
+        <v>0.14634703233333335</v>
       </c>
     </row>
     <row r="192" spans="1:10" x14ac:dyDescent="0.25">
@@ -10520,8 +10533,8 @@
         <v>6.3013699000000006E-2</v>
       </c>
       <c r="J192">
-        <f t="shared" si="5"/>
-        <v>0.72968036566666672</v>
+        <f t="shared" si="10"/>
+        <v>0.14634703233333335</v>
       </c>
     </row>
     <row r="193" spans="1:10" x14ac:dyDescent="0.25">
@@ -10553,8 +10566,8 @@
         <v>6.3013699000000006E-2</v>
       </c>
       <c r="J193">
-        <f t="shared" si="5"/>
-        <v>0.72968036566666672</v>
+        <f t="shared" si="10"/>
+        <v>0.14634703233333335</v>
       </c>
     </row>
     <row r="194" spans="1:10" x14ac:dyDescent="0.25">
@@ -10586,8 +10599,8 @@
         <v>6.3013699000000006E-2</v>
       </c>
       <c r="J194">
-        <f t="shared" si="5"/>
-        <v>0.72968036566666672</v>
+        <f t="shared" si="10"/>
+        <v>0.14634703233333335</v>
       </c>
     </row>
     <row r="195" spans="1:10" x14ac:dyDescent="0.25">
@@ -10619,8 +10632,8 @@
         <v>6.3013699000000006E-2</v>
       </c>
       <c r="J195">
-        <f t="shared" ref="J195:J258" si="6">IF(A195="R. diluvianum", I195, IF(A195="A. incurva", MOD(I195-4/12, 1), MOD(I195-1/12, 1)))</f>
-        <v>0.72968036566666672</v>
+        <f t="shared" ref="J195:J258" si="11">IF(A195="R. diluvianum", MOD(I195+5/12, 1), IF(A195="A. incurva", MOD(I195+1/12, 1), MOD(I195+4/12, 1)))</f>
+        <v>0.14634703233333335</v>
       </c>
     </row>
     <row r="196" spans="1:10" x14ac:dyDescent="0.25">
@@ -10652,8 +10665,8 @@
         <v>6.3013699000000006E-2</v>
       </c>
       <c r="J196">
-        <f t="shared" si="6"/>
-        <v>0.72968036566666672</v>
+        <f t="shared" si="11"/>
+        <v>0.14634703233333335</v>
       </c>
     </row>
     <row r="197" spans="1:10" x14ac:dyDescent="0.25">
@@ -10685,8 +10698,8 @@
         <v>0.33150684899999999</v>
       </c>
       <c r="J197">
-        <f t="shared" si="6"/>
-        <v>0.99817351566666668</v>
+        <f t="shared" si="11"/>
+        <v>0.41484018233333331</v>
       </c>
     </row>
     <row r="198" spans="1:10" x14ac:dyDescent="0.25">
@@ -10718,8 +10731,8 @@
         <v>0.33150684899999999</v>
       </c>
       <c r="J198">
-        <f t="shared" si="6"/>
-        <v>0.99817351566666668</v>
+        <f t="shared" si="11"/>
+        <v>0.41484018233333331</v>
       </c>
     </row>
     <row r="199" spans="1:10" x14ac:dyDescent="0.25">
@@ -10751,8 +10764,8 @@
         <v>0.67397260299999995</v>
       </c>
       <c r="J199">
-        <f t="shared" si="6"/>
-        <v>0.34063926966666663</v>
+        <f t="shared" si="11"/>
+        <v>0.75730593633333332</v>
       </c>
     </row>
     <row r="200" spans="1:10" x14ac:dyDescent="0.25">
@@ -10784,8 +10797,8 @@
         <v>0.67397260299999995</v>
       </c>
       <c r="J200">
-        <f t="shared" si="6"/>
-        <v>0.34063926966666663</v>
+        <f t="shared" si="11"/>
+        <v>0.75730593633333332</v>
       </c>
     </row>
     <row r="201" spans="1:10" x14ac:dyDescent="0.25">
@@ -10817,8 +10830,8 @@
         <v>0.93698630100000002</v>
       </c>
       <c r="J201">
-        <f t="shared" si="6"/>
-        <v>0.60365296766666665</v>
+        <f t="shared" si="11"/>
+        <v>2.0319634333333392E-2</v>
       </c>
     </row>
     <row r="202" spans="1:10" x14ac:dyDescent="0.25">
@@ -10850,8 +10863,8 @@
         <v>0.93698630100000002</v>
       </c>
       <c r="J202">
-        <f t="shared" si="6"/>
-        <v>0.60365296766666665</v>
+        <f t="shared" si="11"/>
+        <v>2.0319634333333392E-2</v>
       </c>
     </row>
     <row r="203" spans="1:10" x14ac:dyDescent="0.25">
@@ -10883,8 +10896,8 @@
         <v>4.3835616000000001E-2</v>
       </c>
       <c r="J203">
-        <f t="shared" si="6"/>
-        <v>0.71050228266666671</v>
+        <f t="shared" si="11"/>
+        <v>0.12716894933333334</v>
       </c>
     </row>
     <row r="204" spans="1:10" x14ac:dyDescent="0.25">
@@ -10916,8 +10929,8 @@
         <v>4.3835616000000001E-2</v>
       </c>
       <c r="J204">
-        <f t="shared" si="6"/>
-        <v>0.71050228266666671</v>
+        <f t="shared" si="11"/>
+        <v>0.12716894933333334</v>
       </c>
     </row>
     <row r="205" spans="1:10" x14ac:dyDescent="0.25">
@@ -10949,8 +10962,8 @@
         <v>0.12602739700000001</v>
       </c>
       <c r="J205">
-        <f t="shared" si="6"/>
-        <v>0.79269406366666673</v>
+        <f t="shared" si="11"/>
+        <v>0.20936073033333336</v>
       </c>
     </row>
     <row r="206" spans="1:10" x14ac:dyDescent="0.25">
@@ -10982,8 +10995,8 @@
         <v>0.12602739700000001</v>
       </c>
       <c r="J206">
-        <f t="shared" si="6"/>
-        <v>0.79269406366666673</v>
+        <f t="shared" si="11"/>
+        <v>0.20936073033333336</v>
       </c>
     </row>
     <row r="207" spans="1:10" x14ac:dyDescent="0.25">
@@ -11015,8 +11028,8 @@
         <v>0.19726027400000001</v>
       </c>
       <c r="J207">
-        <f t="shared" si="6"/>
-        <v>0.86392694066666675</v>
+        <f t="shared" si="11"/>
+        <v>0.28059360733333333</v>
       </c>
     </row>
     <row r="208" spans="1:10" x14ac:dyDescent="0.25">
@@ -11048,8 +11061,8 @@
         <v>0.19726027400000001</v>
       </c>
       <c r="J208">
-        <f t="shared" si="6"/>
-        <v>0.86392694066666675</v>
+        <f t="shared" si="11"/>
+        <v>0.28059360733333333</v>
       </c>
     </row>
     <row r="209" spans="1:10" x14ac:dyDescent="0.25">
@@ -11081,8 +11094,8 @@
         <v>0.26301369899999999</v>
       </c>
       <c r="J209">
-        <f t="shared" si="6"/>
-        <v>0.92968036566666667</v>
+        <f t="shared" si="11"/>
+        <v>0.3463470323333333</v>
       </c>
     </row>
     <row r="210" spans="1:10" x14ac:dyDescent="0.25">
@@ -11114,8 +11127,8 @@
         <v>0.26301369899999999</v>
       </c>
       <c r="J210">
-        <f t="shared" si="6"/>
-        <v>0.92968036566666667</v>
+        <f t="shared" si="11"/>
+        <v>0.3463470323333333</v>
       </c>
     </row>
     <row r="211" spans="1:10" x14ac:dyDescent="0.25">
@@ -11147,8 +11160,8 @@
         <v>0.326027397</v>
       </c>
       <c r="J211">
-        <f t="shared" si="6"/>
-        <v>0.99269406366666668</v>
+        <f t="shared" si="11"/>
+        <v>0.40936073033333331</v>
       </c>
     </row>
     <row r="212" spans="1:10" x14ac:dyDescent="0.25">
@@ -11180,8 +11193,8 @@
         <v>0.39452054800000003</v>
       </c>
       <c r="J212">
-        <f t="shared" si="6"/>
-        <v>6.1187214666666712E-2</v>
+        <f t="shared" si="11"/>
+        <v>0.47785388133333334</v>
       </c>
     </row>
     <row r="213" spans="1:10" x14ac:dyDescent="0.25">
@@ -11213,8 +11226,8 @@
         <v>0.39452054800000003</v>
       </c>
       <c r="J213">
-        <f t="shared" si="6"/>
-        <v>6.1187214666666712E-2</v>
+        <f t="shared" si="11"/>
+        <v>0.47785388133333334</v>
       </c>
     </row>
     <row r="214" spans="1:10" x14ac:dyDescent="0.25">
@@ -11246,8 +11259,8 @@
         <v>0.97260274000000002</v>
       </c>
       <c r="J214">
-        <f t="shared" si="6"/>
-        <v>0.63926940666666665</v>
+        <f t="shared" si="11"/>
+        <v>5.5936073333333391E-2</v>
       </c>
     </row>
     <row r="215" spans="1:10" x14ac:dyDescent="0.25">
@@ -11279,8 +11292,8 @@
         <v>0.97260274000000002</v>
       </c>
       <c r="J215">
-        <f t="shared" si="6"/>
-        <v>0.63926940666666665</v>
+        <f t="shared" si="11"/>
+        <v>5.5936073333333391E-2</v>
       </c>
     </row>
     <row r="216" spans="1:10" x14ac:dyDescent="0.25">
@@ -11312,8 +11325,8 @@
         <v>1.0958904E-2</v>
       </c>
       <c r="J216">
-        <f t="shared" si="6"/>
-        <v>0.67762557066666673</v>
+        <f t="shared" si="11"/>
+        <v>9.4292237333333334E-2</v>
       </c>
     </row>
     <row r="217" spans="1:10" x14ac:dyDescent="0.25">
@@ -11345,8 +11358,8 @@
         <v>1.0958904E-2</v>
       </c>
       <c r="J217">
-        <f t="shared" si="6"/>
-        <v>0.67762557066666673</v>
+        <f t="shared" si="11"/>
+        <v>9.4292237333333334E-2</v>
       </c>
     </row>
     <row r="218" spans="1:10" x14ac:dyDescent="0.25">
@@ -11378,8 +11391,8 @@
         <v>4.6575341999999999E-2</v>
       </c>
       <c r="J218">
-        <f t="shared" si="6"/>
-        <v>0.71324200866666665</v>
+        <f t="shared" si="11"/>
+        <v>0.12990867533333333</v>
       </c>
     </row>
     <row r="219" spans="1:10" x14ac:dyDescent="0.25">
@@ -11411,8 +11424,8 @@
         <v>4.6575341999999999E-2</v>
       </c>
       <c r="J219">
-        <f t="shared" si="6"/>
-        <v>0.71324200866666665</v>
+        <f t="shared" si="11"/>
+        <v>0.12990867533333333</v>
       </c>
     </row>
     <row r="220" spans="1:10" x14ac:dyDescent="0.25">
@@ -11444,8 +11457,8 @@
         <v>8.7671233000000001E-2</v>
       </c>
       <c r="J220">
-        <f t="shared" si="6"/>
-        <v>0.75433789966666676</v>
+        <f t="shared" si="11"/>
+        <v>0.17100456633333333</v>
       </c>
     </row>
     <row r="221" spans="1:10" x14ac:dyDescent="0.25">
@@ -11477,8 +11490,8 @@
         <v>8.7671233000000001E-2</v>
       </c>
       <c r="J221">
-        <f t="shared" si="6"/>
-        <v>0.75433789966666676</v>
+        <f t="shared" si="11"/>
+        <v>0.17100456633333333</v>
       </c>
     </row>
     <row r="222" spans="1:10" x14ac:dyDescent="0.25">
@@ -11510,8 +11523,8 @@
         <v>0.12602739700000001</v>
       </c>
       <c r="J222">
-        <f t="shared" si="6"/>
-        <v>0.79269406366666673</v>
+        <f t="shared" si="11"/>
+        <v>0.20936073033333336</v>
       </c>
     </row>
     <row r="223" spans="1:10" x14ac:dyDescent="0.25">
@@ -11543,8 +11556,8 @@
         <v>0.12602739700000001</v>
       </c>
       <c r="J223">
-        <f t="shared" si="6"/>
-        <v>0.79269406366666673</v>
+        <f t="shared" si="11"/>
+        <v>0.20936073033333336</v>
       </c>
     </row>
     <row r="224" spans="1:10" x14ac:dyDescent="0.25">
@@ -11576,8 +11589,8 @@
         <v>0.16986301400000001</v>
       </c>
       <c r="J224">
-        <f t="shared" si="6"/>
-        <v>0.83652968066666666</v>
+        <f t="shared" si="11"/>
+        <v>0.25319634733333335</v>
       </c>
     </row>
     <row r="225" spans="1:10" x14ac:dyDescent="0.25">
@@ -11609,8 +11622,8 @@
         <v>0.16986301400000001</v>
       </c>
       <c r="J225">
-        <f t="shared" si="6"/>
-        <v>0.83652968066666666</v>
+        <f t="shared" si="11"/>
+        <v>0.25319634733333335</v>
       </c>
     </row>
     <row r="226" spans="1:10" x14ac:dyDescent="0.25">
@@ -11642,8 +11655,8 @@
         <v>0.216438356</v>
       </c>
       <c r="J226">
-        <f t="shared" si="6"/>
-        <v>0.88310502266666668</v>
+        <f t="shared" si="11"/>
+        <v>0.29977168933333331</v>
       </c>
     </row>
     <row r="227" spans="1:10" x14ac:dyDescent="0.25">
@@ -11675,8 +11688,8 @@
         <v>0.216438356</v>
       </c>
       <c r="J227">
-        <f t="shared" si="6"/>
-        <v>0.88310502266666668</v>
+        <f t="shared" si="11"/>
+        <v>0.29977168933333331</v>
       </c>
     </row>
     <row r="228" spans="1:10" x14ac:dyDescent="0.25">
@@ -11708,8 +11721,8 @@
         <v>0.26575342499999999</v>
       </c>
       <c r="J228">
-        <f t="shared" si="6"/>
-        <v>0.93242009166666673</v>
+        <f t="shared" si="11"/>
+        <v>0.3490867583333333</v>
       </c>
     </row>
     <row r="229" spans="1:10" x14ac:dyDescent="0.25">
@@ -11741,8 +11754,8 @@
         <v>0.26575342499999999</v>
       </c>
       <c r="J229">
-        <f t="shared" si="6"/>
-        <v>0.93242009166666673</v>
+        <f t="shared" si="11"/>
+        <v>0.3490867583333333</v>
       </c>
     </row>
     <row r="230" spans="1:10" x14ac:dyDescent="0.25">
@@ -11774,8 +11787,8 @@
         <v>0.326027397</v>
       </c>
       <c r="J230">
-        <f t="shared" si="6"/>
-        <v>0.99269406366666668</v>
+        <f t="shared" si="11"/>
+        <v>0.40936073033333331</v>
       </c>
     </row>
     <row r="231" spans="1:10" x14ac:dyDescent="0.25">
@@ -11807,8 +11820,8 @@
         <v>0.326027397</v>
       </c>
       <c r="J231">
-        <f t="shared" si="6"/>
-        <v>0.99269406366666668</v>
+        <f t="shared" si="11"/>
+        <v>0.40936073033333331</v>
       </c>
     </row>
     <row r="232" spans="1:10" x14ac:dyDescent="0.25">
@@ -11840,8 +11853,8 @@
         <v>0.40273972600000002</v>
       </c>
       <c r="J232">
-        <f t="shared" si="6"/>
-        <v>6.9406392666666705E-2</v>
+        <f t="shared" si="11"/>
+        <v>0.48607305933333333</v>
       </c>
     </row>
     <row r="233" spans="1:10" x14ac:dyDescent="0.25">
@@ -11873,8 +11886,8 @@
         <v>0.40273972600000002</v>
       </c>
       <c r="J233">
-        <f t="shared" si="6"/>
-        <v>6.9406392666666705E-2</v>
+        <f t="shared" si="11"/>
+        <v>0.48607305933333333</v>
       </c>
     </row>
     <row r="234" spans="1:10" x14ac:dyDescent="0.25">
@@ -11906,8 +11919,8 @@
         <v>0.57260274</v>
       </c>
       <c r="J234">
-        <f t="shared" si="6"/>
-        <v>0.23926940666666668</v>
+        <f t="shared" si="11"/>
+        <v>0.65593607333333337</v>
       </c>
     </row>
     <row r="235" spans="1:10" x14ac:dyDescent="0.25">
@@ -11939,8 +11952,8 @@
         <v>0.57260274</v>
       </c>
       <c r="J235">
-        <f t="shared" si="6"/>
-        <v>0.23926940666666668</v>
+        <f t="shared" si="11"/>
+        <v>0.65593607333333337</v>
       </c>
     </row>
     <row r="236" spans="1:10" x14ac:dyDescent="0.25">
@@ -11972,8 +11985,8 @@
         <v>0.97260274000000002</v>
       </c>
       <c r="J236">
-        <f t="shared" si="6"/>
-        <v>0.63926940666666665</v>
+        <f t="shared" si="11"/>
+        <v>5.5936073333333391E-2</v>
       </c>
     </row>
     <row r="237" spans="1:10" x14ac:dyDescent="0.25">
@@ -12005,8 +12018,8 @@
         <v>0.97260274000000002</v>
       </c>
       <c r="J237">
-        <f t="shared" si="6"/>
-        <v>0.63926940666666665</v>
+        <f t="shared" si="11"/>
+        <v>5.5936073333333391E-2</v>
       </c>
     </row>
     <row r="238" spans="1:10" x14ac:dyDescent="0.25">
@@ -12038,8 +12051,8 @@
         <v>0.120547945</v>
       </c>
       <c r="J238">
-        <f t="shared" si="6"/>
-        <v>3.7214611666666675E-2</v>
+        <f t="shared" si="11"/>
+        <v>0.4538812783333333</v>
       </c>
     </row>
     <row r="239" spans="1:10" x14ac:dyDescent="0.25">
@@ -12071,8 +12084,8 @@
         <v>0.22191780799999999</v>
       </c>
       <c r="J239">
-        <f t="shared" si="6"/>
-        <v>0.13858447466666668</v>
+        <f t="shared" si="11"/>
+        <v>0.55525114133333331</v>
       </c>
     </row>
     <row r="240" spans="1:10" x14ac:dyDescent="0.25">
@@ -12104,8 +12117,8 @@
         <v>0.22739725999999999</v>
       </c>
       <c r="J240">
-        <f t="shared" si="6"/>
-        <v>0.14406392666666668</v>
+        <f t="shared" si="11"/>
+        <v>0.5607305933333333</v>
       </c>
     </row>
     <row r="241" spans="1:10" x14ac:dyDescent="0.25">
@@ -12137,8 +12150,8 @@
         <v>0.22739725999999999</v>
       </c>
       <c r="J241">
-        <f t="shared" si="6"/>
-        <v>0.14406392666666668</v>
+        <f t="shared" si="11"/>
+        <v>0.5607305933333333</v>
       </c>
     </row>
     <row r="242" spans="1:10" x14ac:dyDescent="0.25">
@@ -12170,8 +12183,8 @@
         <v>0.32876712299999999</v>
       </c>
       <c r="J242">
-        <f t="shared" si="6"/>
-        <v>0.24543378966666668</v>
+        <f t="shared" si="11"/>
+        <v>0.66210045633333325</v>
       </c>
     </row>
     <row r="243" spans="1:10" x14ac:dyDescent="0.25">
@@ -12203,8 +12216,8 @@
         <v>0.32876712299999999</v>
       </c>
       <c r="J243">
-        <f t="shared" si="6"/>
-        <v>0.24543378966666668</v>
+        <f t="shared" si="11"/>
+        <v>0.66210045633333325</v>
       </c>
     </row>
     <row r="244" spans="1:10" x14ac:dyDescent="0.25">
@@ -12236,8 +12249,8 @@
         <v>0.32876712299999999</v>
       </c>
       <c r="J244">
-        <f t="shared" si="6"/>
-        <v>0.24543378966666668</v>
+        <f t="shared" si="11"/>
+        <v>0.66210045633333325</v>
       </c>
     </row>
     <row r="245" spans="1:10" x14ac:dyDescent="0.25">
@@ -12269,8 +12282,8 @@
         <v>0.59452054799999998</v>
       </c>
       <c r="J245">
-        <f t="shared" si="6"/>
-        <v>0.51118721466666661</v>
+        <f t="shared" si="11"/>
+        <v>0.92785388133333324</v>
       </c>
     </row>
     <row r="246" spans="1:10" x14ac:dyDescent="0.25">
@@ -12302,8 +12315,8 @@
         <v>0.59452054799999998</v>
       </c>
       <c r="J246">
-        <f t="shared" si="6"/>
-        <v>0.51118721466666661</v>
+        <f t="shared" si="11"/>
+        <v>0.92785388133333324</v>
       </c>
     </row>
     <row r="247" spans="1:10" x14ac:dyDescent="0.25">
@@ -12335,8 +12348,8 @@
         <v>0.59452054799999998</v>
       </c>
       <c r="J247">
-        <f t="shared" si="6"/>
-        <v>0.51118721466666661</v>
+        <f t="shared" si="11"/>
+        <v>0.92785388133333324</v>
       </c>
     </row>
     <row r="248" spans="1:10" x14ac:dyDescent="0.25">
@@ -12368,8 +12381,8 @@
         <v>0.59452054799999998</v>
       </c>
       <c r="J248">
-        <f t="shared" si="6"/>
-        <v>0.51118721466666661</v>
+        <f t="shared" si="11"/>
+        <v>0.92785388133333324</v>
       </c>
     </row>
     <row r="249" spans="1:10" x14ac:dyDescent="0.25">
@@ -12401,8 +12414,8 @@
         <v>0.59452054799999998</v>
       </c>
       <c r="J249">
-        <f t="shared" si="6"/>
-        <v>0.51118721466666661</v>
+        <f t="shared" si="11"/>
+        <v>0.92785388133333324</v>
       </c>
     </row>
     <row r="250" spans="1:10" x14ac:dyDescent="0.25">
@@ -12434,8 +12447,8 @@
         <v>0.84931506800000001</v>
       </c>
       <c r="J250">
-        <f t="shared" si="6"/>
-        <v>0.76598173466666664</v>
+        <f t="shared" si="11"/>
+        <v>0.18264840133333338</v>
       </c>
     </row>
     <row r="251" spans="1:10" x14ac:dyDescent="0.25">
@@ -12467,8 +12480,8 @@
         <v>0.84931506800000001</v>
       </c>
       <c r="J251">
-        <f t="shared" si="6"/>
-        <v>0.76598173466666664</v>
+        <f t="shared" si="11"/>
+        <v>0.18264840133333338</v>
       </c>
     </row>
     <row r="252" spans="1:10" x14ac:dyDescent="0.25">
@@ -12500,8 +12513,8 @@
         <v>0.97534246599999996</v>
       </c>
       <c r="J252">
-        <f t="shared" si="6"/>
-        <v>0.89200913266666659</v>
+        <f t="shared" si="11"/>
+        <v>0.30867579933333333</v>
       </c>
     </row>
     <row r="253" spans="1:10" x14ac:dyDescent="0.25">
@@ -12533,8 +12546,8 @@
         <v>0</v>
       </c>
       <c r="J253">
-        <f t="shared" si="6"/>
-        <v>0.91666666666666663</v>
+        <f t="shared" si="11"/>
+        <v>0.33333333333333331</v>
       </c>
     </row>
     <row r="254" spans="1:10" x14ac:dyDescent="0.25">
@@ -12566,8 +12579,8 @@
         <v>0</v>
       </c>
       <c r="J254">
-        <f t="shared" si="6"/>
-        <v>0.91666666666666663</v>
+        <f t="shared" si="11"/>
+        <v>0.33333333333333331</v>
       </c>
     </row>
     <row r="255" spans="1:10" x14ac:dyDescent="0.25">
@@ -12599,8 +12612,8 @@
         <v>0</v>
       </c>
       <c r="J255">
-        <f t="shared" si="6"/>
-        <v>0.91666666666666663</v>
+        <f t="shared" si="11"/>
+        <v>0.33333333333333331</v>
       </c>
     </row>
     <row r="256" spans="1:10" x14ac:dyDescent="0.25">
@@ -12632,8 +12645,8 @@
         <v>9.5890410999999995E-2</v>
       </c>
       <c r="J256">
-        <f t="shared" si="6"/>
-        <v>1.2557077666666666E-2</v>
+        <f t="shared" si="11"/>
+        <v>0.42922374433333332</v>
       </c>
     </row>
     <row r="257" spans="1:10" x14ac:dyDescent="0.25">
@@ -12665,8 +12678,8 @@
         <v>0.120547945</v>
       </c>
       <c r="J257">
-        <f t="shared" si="6"/>
-        <v>3.7214611666666675E-2</v>
+        <f t="shared" si="11"/>
+        <v>0.4538812783333333</v>
       </c>
     </row>
     <row r="258" spans="1:10" x14ac:dyDescent="0.25">
@@ -12698,8 +12711,8 @@
         <v>0.22739725999999999</v>
       </c>
       <c r="J258">
-        <f t="shared" si="6"/>
-        <v>0.14406392666666668</v>
+        <f t="shared" si="11"/>
+        <v>0.5607305933333333</v>
       </c>
     </row>
     <row r="259" spans="1:10" x14ac:dyDescent="0.25">
@@ -12731,8 +12744,8 @@
         <v>0.22739725999999999</v>
       </c>
       <c r="J259">
-        <f t="shared" ref="J259:J322" si="7">IF(A259="R. diluvianum", I259, IF(A259="A. incurva", MOD(I259-4/12, 1), MOD(I259-1/12, 1)))</f>
-        <v>0.14406392666666668</v>
+        <f t="shared" ref="J259:J322" si="12">IF(A259="R. diluvianum", MOD(I259+5/12, 1), IF(A259="A. incurva", MOD(I259+1/12, 1), MOD(I259+4/12, 1)))</f>
+        <v>0.5607305933333333</v>
       </c>
     </row>
     <row r="260" spans="1:10" x14ac:dyDescent="0.25">
@@ -12764,8 +12777,8 @@
         <v>0.30136986300000002</v>
       </c>
       <c r="J260">
-        <f t="shared" si="7"/>
-        <v>0.2180365296666667</v>
+        <f t="shared" si="12"/>
+        <v>0.63470319633333339</v>
       </c>
     </row>
     <row r="261" spans="1:10" x14ac:dyDescent="0.25">
@@ -12797,8 +12810,8 @@
         <v>0.32876712299999999</v>
       </c>
       <c r="J261">
-        <f t="shared" si="7"/>
-        <v>0.24543378966666668</v>
+        <f t="shared" si="12"/>
+        <v>0.66210045633333325</v>
       </c>
     </row>
     <row r="262" spans="1:10" x14ac:dyDescent="0.25">
@@ -12830,8 +12843,8 @@
         <v>0.32876712299999999</v>
       </c>
       <c r="J262">
-        <f t="shared" si="7"/>
-        <v>0.24543378966666668</v>
+        <f t="shared" si="12"/>
+        <v>0.66210045633333325</v>
       </c>
     </row>
     <row r="263" spans="1:10" x14ac:dyDescent="0.25">
@@ -12863,8 +12876,8 @@
         <v>0.32876712299999999</v>
       </c>
       <c r="J263">
-        <f t="shared" si="7"/>
-        <v>0.24543378966666668</v>
+        <f t="shared" si="12"/>
+        <v>0.66210045633333325</v>
       </c>
     </row>
     <row r="264" spans="1:10" x14ac:dyDescent="0.25">
@@ -12896,8 +12909,8 @@
         <v>0.59452054799999998</v>
       </c>
       <c r="J264">
-        <f t="shared" si="7"/>
-        <v>0.51118721466666661</v>
+        <f t="shared" si="12"/>
+        <v>0.92785388133333324</v>
       </c>
     </row>
     <row r="265" spans="1:10" x14ac:dyDescent="0.25">
@@ -12929,8 +12942,8 @@
         <v>0.59452054799999998</v>
       </c>
       <c r="J265">
-        <f t="shared" si="7"/>
-        <v>0.51118721466666661</v>
+        <f t="shared" si="12"/>
+        <v>0.92785388133333324</v>
       </c>
     </row>
     <row r="266" spans="1:10" x14ac:dyDescent="0.25">
@@ -12962,8 +12975,8 @@
         <v>0.59452054799999998</v>
       </c>
       <c r="J266">
-        <f t="shared" si="7"/>
-        <v>0.51118721466666661</v>
+        <f t="shared" si="12"/>
+        <v>0.92785388133333324</v>
       </c>
     </row>
     <row r="267" spans="1:10" x14ac:dyDescent="0.25">
@@ -12995,8 +13008,8 @@
         <v>0.59452054799999998</v>
       </c>
       <c r="J267">
-        <f t="shared" si="7"/>
-        <v>0.51118721466666661</v>
+        <f t="shared" si="12"/>
+        <v>0.92785388133333324</v>
       </c>
     </row>
     <row r="268" spans="1:10" x14ac:dyDescent="0.25">
@@ -13028,8 +13041,8 @@
         <v>0.780821918</v>
       </c>
       <c r="J268">
-        <f t="shared" si="7"/>
-        <v>0.69748858466666663</v>
+        <f t="shared" si="12"/>
+        <v>0.11415525133333326</v>
       </c>
     </row>
     <row r="269" spans="1:10" x14ac:dyDescent="0.25">
@@ -13061,8 +13074,8 @@
         <v>0.85205479500000003</v>
       </c>
       <c r="J269">
-        <f t="shared" si="7"/>
-        <v>0.76872146166666666</v>
+        <f t="shared" si="12"/>
+        <v>0.1853881283333334</v>
       </c>
     </row>
     <row r="270" spans="1:10" x14ac:dyDescent="0.25">
@@ -13094,8 +13107,8 @@
         <v>0.85205479500000003</v>
       </c>
       <c r="J270">
-        <f t="shared" si="7"/>
-        <v>0.76872146166666666</v>
+        <f t="shared" si="12"/>
+        <v>0.1853881283333334</v>
       </c>
     </row>
     <row r="271" spans="1:10" x14ac:dyDescent="0.25">
@@ -13127,8 +13140,8 @@
         <v>0.85205479500000003</v>
       </c>
       <c r="J271">
-        <f t="shared" si="7"/>
-        <v>0.76872146166666666</v>
+        <f t="shared" si="12"/>
+        <v>0.1853881283333334</v>
       </c>
     </row>
     <row r="272" spans="1:10" x14ac:dyDescent="0.25">
@@ -13160,8 +13173,8 @@
         <v>0.85205479500000003</v>
       </c>
       <c r="J272">
-        <f t="shared" si="7"/>
-        <v>0.76872146166666666</v>
+        <f t="shared" si="12"/>
+        <v>0.1853881283333334</v>
       </c>
     </row>
     <row r="273" spans="1:10" x14ac:dyDescent="0.25">
@@ -13193,8 +13206,8 @@
         <v>0.85205479500000003</v>
       </c>
       <c r="J273">
-        <f t="shared" si="7"/>
-        <v>0.76872146166666666</v>
+        <f t="shared" si="12"/>
+        <v>0.1853881283333334</v>
       </c>
     </row>
     <row r="274" spans="1:10" x14ac:dyDescent="0.25">
@@ -13226,8 +13239,8 @@
         <v>0.91780821899999998</v>
       </c>
       <c r="J274">
-        <f t="shared" si="7"/>
-        <v>0.83447488566666661</v>
+        <f t="shared" si="12"/>
+        <v>0.25114155233333335</v>
       </c>
     </row>
     <row r="275" spans="1:10" x14ac:dyDescent="0.25">
@@ -13259,8 +13272,8 @@
         <v>0.91780821899999998</v>
       </c>
       <c r="J275">
-        <f t="shared" si="7"/>
-        <v>0.83447488566666661</v>
+        <f t="shared" si="12"/>
+        <v>0.25114155233333335</v>
       </c>
     </row>
     <row r="276" spans="1:10" x14ac:dyDescent="0.25">
@@ -13292,8 +13305,8 @@
         <v>0.91780821899999998</v>
       </c>
       <c r="J276">
-        <f t="shared" si="7"/>
-        <v>0.83447488566666661</v>
+        <f t="shared" si="12"/>
+        <v>0.25114155233333335</v>
       </c>
     </row>
     <row r="277" spans="1:10" x14ac:dyDescent="0.25">
@@ -13325,8 +13338,8 @@
         <v>0.91780821899999998</v>
       </c>
       <c r="J277">
-        <f t="shared" si="7"/>
-        <v>0.83447488566666661</v>
+        <f t="shared" si="12"/>
+        <v>0.25114155233333335</v>
       </c>
     </row>
     <row r="278" spans="1:10" x14ac:dyDescent="0.25">
@@ -13358,8 +13371,8 @@
         <v>0.95068493200000004</v>
       </c>
       <c r="J278">
-        <f t="shared" si="7"/>
-        <v>0.86735159866666667</v>
+        <f t="shared" si="12"/>
+        <v>0.28401826533333341</v>
       </c>
     </row>
     <row r="279" spans="1:10" x14ac:dyDescent="0.25">
@@ -13391,8 +13404,8 @@
         <v>0.97260274000000002</v>
       </c>
       <c r="J279">
-        <f t="shared" si="7"/>
-        <v>0.88926940666666665</v>
+        <f t="shared" si="12"/>
+        <v>0.30593607333333339</v>
       </c>
     </row>
     <row r="280" spans="1:10" x14ac:dyDescent="0.25">
@@ -13424,8 +13437,8 @@
         <v>1.6438356000000001E-2</v>
       </c>
       <c r="J280">
-        <f t="shared" si="7"/>
-        <v>0.93310502266666662</v>
+        <f t="shared" si="12"/>
+        <v>0.3497716893333333</v>
       </c>
     </row>
     <row r="281" spans="1:10" x14ac:dyDescent="0.25">
@@ -13457,8 +13470,8 @@
         <v>1.6438356000000001E-2</v>
       </c>
       <c r="J281">
-        <f t="shared" si="7"/>
-        <v>0.93310502266666662</v>
+        <f t="shared" si="12"/>
+        <v>0.3497716893333333</v>
       </c>
     </row>
     <row r="282" spans="1:10" x14ac:dyDescent="0.25">
@@ -13490,8 +13503,8 @@
         <v>1.6438356000000001E-2</v>
       </c>
       <c r="J282">
-        <f t="shared" si="7"/>
-        <v>0.93310502266666662</v>
+        <f t="shared" si="12"/>
+        <v>0.3497716893333333</v>
       </c>
     </row>
     <row r="283" spans="1:10" x14ac:dyDescent="0.25">
@@ -13523,8 +13536,8 @@
         <v>5.7534246999999997E-2</v>
       </c>
       <c r="J283">
-        <f t="shared" si="7"/>
-        <v>0.97420091366666672</v>
+        <f t="shared" si="12"/>
+        <v>0.3908675803333333</v>
       </c>
     </row>
     <row r="284" spans="1:10" x14ac:dyDescent="0.25">
@@ -13556,8 +13569,8 @@
         <v>5.7534246999999997E-2</v>
       </c>
       <c r="J284">
-        <f t="shared" si="7"/>
-        <v>0.97420091366666672</v>
+        <f t="shared" si="12"/>
+        <v>0.3908675803333333</v>
       </c>
     </row>
     <row r="285" spans="1:10" x14ac:dyDescent="0.25">
@@ -13589,8 +13602,8 @@
         <v>5.7534246999999997E-2</v>
       </c>
       <c r="J285">
-        <f t="shared" si="7"/>
-        <v>0.97420091366666672</v>
+        <f t="shared" si="12"/>
+        <v>0.3908675803333333</v>
       </c>
     </row>
     <row r="286" spans="1:10" x14ac:dyDescent="0.25">
@@ -13622,8 +13635,8 @@
         <v>7.9452054999999994E-2</v>
       </c>
       <c r="J286">
-        <f t="shared" si="7"/>
-        <v>0.99611872166666671</v>
+        <f t="shared" si="12"/>
+        <v>0.41278538833333334</v>
       </c>
     </row>
     <row r="287" spans="1:10" x14ac:dyDescent="0.25">
@@ -13655,8 +13668,8 @@
         <v>9.8630137000000007E-2</v>
       </c>
       <c r="J287">
-        <f t="shared" si="7"/>
-        <v>1.5296803666666678E-2</v>
+        <f t="shared" si="12"/>
+        <v>0.43196347033333332</v>
       </c>
     </row>
     <row r="288" spans="1:10" x14ac:dyDescent="0.25">
@@ -13688,8 +13701,8 @@
         <v>9.8630137000000007E-2</v>
       </c>
       <c r="J288">
-        <f t="shared" si="7"/>
-        <v>1.5296803666666678E-2</v>
+        <f t="shared" si="12"/>
+        <v>0.43196347033333332</v>
       </c>
     </row>
     <row r="289" spans="1:10" x14ac:dyDescent="0.25">
@@ -13721,8 +13734,8 @@
         <v>9.8630137000000007E-2</v>
       </c>
       <c r="J289">
-        <f t="shared" si="7"/>
-        <v>1.5296803666666678E-2</v>
+        <f t="shared" si="12"/>
+        <v>0.43196347033333332</v>
       </c>
     </row>
     <row r="290" spans="1:10" x14ac:dyDescent="0.25">
@@ -13754,8 +13767,8 @@
         <v>9.8630137000000007E-2</v>
       </c>
       <c r="J290">
-        <f t="shared" si="7"/>
-        <v>1.5296803666666678E-2</v>
+        <f t="shared" si="12"/>
+        <v>0.43196347033333332</v>
       </c>
     </row>
     <row r="291" spans="1:10" x14ac:dyDescent="0.25">
@@ -13787,8 +13800,8 @@
         <v>0.136986301</v>
       </c>
       <c r="J291">
-        <f t="shared" si="7"/>
-        <v>5.3652967666666676E-2</v>
+        <f t="shared" si="12"/>
+        <v>0.47031963433333335</v>
       </c>
     </row>
     <row r="292" spans="1:10" x14ac:dyDescent="0.25">
@@ -13820,8 +13833,8 @@
         <v>0.136986301</v>
       </c>
       <c r="J292">
-        <f t="shared" si="7"/>
-        <v>5.3652967666666676E-2</v>
+        <f t="shared" si="12"/>
+        <v>0.47031963433333335</v>
       </c>
     </row>
     <row r="293" spans="1:10" x14ac:dyDescent="0.25">
@@ -13853,8 +13866,8 @@
         <v>0.136986301</v>
       </c>
       <c r="J293">
-        <f t="shared" si="7"/>
-        <v>5.3652967666666676E-2</v>
+        <f t="shared" si="12"/>
+        <v>0.47031963433333335</v>
       </c>
     </row>
     <row r="294" spans="1:10" x14ac:dyDescent="0.25">
@@ -13886,8 +13899,8 @@
         <v>0.136986301</v>
       </c>
       <c r="J294">
-        <f t="shared" si="7"/>
-        <v>5.3652967666666676E-2</v>
+        <f t="shared" si="12"/>
+        <v>0.47031963433333335</v>
       </c>
     </row>
     <row r="295" spans="1:10" x14ac:dyDescent="0.25">
@@ -13919,8 +13932,8 @@
         <v>0.175342466</v>
       </c>
       <c r="J295">
-        <f t="shared" si="7"/>
-        <v>9.2009132666666674E-2</v>
+        <f t="shared" si="12"/>
+        <v>0.50867579933333329</v>
       </c>
     </row>
     <row r="296" spans="1:10" x14ac:dyDescent="0.25">
@@ -13952,8 +13965,8 @@
         <v>0.175342466</v>
       </c>
       <c r="J296">
-        <f t="shared" si="7"/>
-        <v>9.2009132666666674E-2</v>
+        <f t="shared" si="12"/>
+        <v>0.50867579933333329</v>
       </c>
     </row>
     <row r="297" spans="1:10" x14ac:dyDescent="0.25">
@@ -13985,8 +13998,8 @@
         <v>0.175342466</v>
       </c>
       <c r="J297">
-        <f t="shared" si="7"/>
-        <v>9.2009132666666674E-2</v>
+        <f t="shared" si="12"/>
+        <v>0.50867579933333329</v>
       </c>
     </row>
     <row r="298" spans="1:10" x14ac:dyDescent="0.25">
@@ -14018,8 +14031,8 @@
         <v>0.219178082</v>
       </c>
       <c r="J298">
-        <f t="shared" si="7"/>
-        <v>0.13584474866666668</v>
+        <f t="shared" si="12"/>
+        <v>0.55251141533333326</v>
       </c>
     </row>
     <row r="299" spans="1:10" x14ac:dyDescent="0.25">
@@ -14051,8 +14064,8 @@
         <v>0.219178082</v>
       </c>
       <c r="J299">
-        <f t="shared" si="7"/>
-        <v>0.13584474866666668</v>
+        <f t="shared" si="12"/>
+        <v>0.55251141533333326</v>
       </c>
     </row>
     <row r="300" spans="1:10" x14ac:dyDescent="0.25">
@@ -14084,8 +14097,8 @@
         <v>0.219178082</v>
       </c>
       <c r="J300">
-        <f t="shared" si="7"/>
-        <v>0.13584474866666668</v>
+        <f t="shared" si="12"/>
+        <v>0.55251141533333326</v>
       </c>
     </row>
     <row r="301" spans="1:10" x14ac:dyDescent="0.25">
@@ -14117,8 +14130,8 @@
         <v>0.26301369899999999</v>
       </c>
       <c r="J301">
-        <f t="shared" si="7"/>
-        <v>0.17968036566666667</v>
+        <f t="shared" si="12"/>
+        <v>0.5963470323333333</v>
       </c>
     </row>
     <row r="302" spans="1:10" x14ac:dyDescent="0.25">
@@ -14150,8 +14163,8 @@
         <v>0.26301369899999999</v>
       </c>
       <c r="J302">
-        <f t="shared" si="7"/>
-        <v>0.17968036566666667</v>
+        <f t="shared" si="12"/>
+        <v>0.5963470323333333</v>
       </c>
     </row>
     <row r="303" spans="1:10" x14ac:dyDescent="0.25">
@@ -14183,8 +14196,8 @@
         <v>0.26301369899999999</v>
       </c>
       <c r="J303">
-        <f t="shared" si="7"/>
-        <v>0.17968036566666667</v>
+        <f t="shared" si="12"/>
+        <v>0.5963470323333333</v>
       </c>
     </row>
     <row r="304" spans="1:10" x14ac:dyDescent="0.25">
@@ -14216,8 +14229,8 @@
         <v>0.31506849300000001</v>
       </c>
       <c r="J304">
-        <f t="shared" si="7"/>
-        <v>0.23173515966666669</v>
+        <f t="shared" si="12"/>
+        <v>0.64840182633333332</v>
       </c>
     </row>
     <row r="305" spans="1:10" x14ac:dyDescent="0.25">
@@ -14249,8 +14262,8 @@
         <v>0.31506849300000001</v>
       </c>
       <c r="J305">
-        <f t="shared" si="7"/>
-        <v>0.23173515966666669</v>
+        <f t="shared" si="12"/>
+        <v>0.64840182633333332</v>
       </c>
     </row>
     <row r="306" spans="1:10" x14ac:dyDescent="0.25">
@@ -14282,8 +14295,8 @@
         <v>0.31506849300000001</v>
       </c>
       <c r="J306">
-        <f t="shared" si="7"/>
-        <v>0.23173515966666669</v>
+        <f t="shared" si="12"/>
+        <v>0.64840182633333332</v>
       </c>
     </row>
     <row r="307" spans="1:10" x14ac:dyDescent="0.25">
@@ -14315,8 +14328,8 @@
         <v>0.38082191799999998</v>
       </c>
       <c r="J307">
-        <f t="shared" si="7"/>
-        <v>0.29748858466666667</v>
+        <f t="shared" si="12"/>
+        <v>0.71415525133333335</v>
       </c>
     </row>
     <row r="308" spans="1:10" x14ac:dyDescent="0.25">
@@ -14348,8 +14361,8 @@
         <v>0.38082191799999998</v>
       </c>
       <c r="J308">
-        <f t="shared" si="7"/>
-        <v>0.29748858466666667</v>
+        <f t="shared" si="12"/>
+        <v>0.71415525133333335</v>
       </c>
     </row>
     <row r="309" spans="1:10" x14ac:dyDescent="0.25">
@@ -14381,8 +14394,8 @@
         <v>0.38082191799999998</v>
       </c>
       <c r="J309">
-        <f t="shared" si="7"/>
-        <v>0.29748858466666667</v>
+        <f t="shared" si="12"/>
+        <v>0.71415525133333335</v>
       </c>
     </row>
     <row r="310" spans="1:10" x14ac:dyDescent="0.25">
@@ -14414,8 +14427,8 @@
         <v>0.38082191799999998</v>
       </c>
       <c r="J310">
-        <f t="shared" si="7"/>
-        <v>0.29748858466666667</v>
+        <f t="shared" si="12"/>
+        <v>0.71415525133333335</v>
       </c>
     </row>
     <row r="311" spans="1:10" x14ac:dyDescent="0.25">
@@ -14447,8 +14460,8 @@
         <v>0.38082191799999998</v>
       </c>
       <c r="J311">
-        <f t="shared" si="7"/>
-        <v>0.29748858466666667</v>
+        <f t="shared" si="12"/>
+        <v>0.71415525133333335</v>
       </c>
     </row>
     <row r="312" spans="1:10" x14ac:dyDescent="0.25">
@@ -14480,8 +14493,8 @@
         <v>0.38082191799999998</v>
       </c>
       <c r="J312">
-        <f t="shared" si="7"/>
-        <v>0.29748858466666667</v>
+        <f t="shared" si="12"/>
+        <v>0.71415525133333335</v>
       </c>
     </row>
     <row r="313" spans="1:10" x14ac:dyDescent="0.25">
@@ -14513,8 +14526,8 @@
         <v>0.50684931499999997</v>
       </c>
       <c r="J313">
-        <f t="shared" si="7"/>
-        <v>0.42351598166666665</v>
+        <f t="shared" si="12"/>
+        <v>0.84018264833333323</v>
       </c>
     </row>
     <row r="314" spans="1:10" x14ac:dyDescent="0.25">
@@ -14546,8 +14559,8 @@
         <v>0.50684931499999997</v>
       </c>
       <c r="J314">
-        <f t="shared" si="7"/>
-        <v>0.42351598166666665</v>
+        <f t="shared" si="12"/>
+        <v>0.84018264833333323</v>
       </c>
     </row>
     <row r="315" spans="1:10" x14ac:dyDescent="0.25">
@@ -14579,8 +14592,8 @@
         <v>0.50684931499999997</v>
       </c>
       <c r="J315">
-        <f t="shared" si="7"/>
-        <v>0.42351598166666665</v>
+        <f t="shared" si="12"/>
+        <v>0.84018264833333323</v>
       </c>
     </row>
     <row r="316" spans="1:10" x14ac:dyDescent="0.25">
@@ -14612,8 +14625,8 @@
         <v>0.50684931499999997</v>
       </c>
       <c r="J316">
-        <f t="shared" si="7"/>
-        <v>0.42351598166666665</v>
+        <f t="shared" si="12"/>
+        <v>0.84018264833333323</v>
       </c>
     </row>
     <row r="317" spans="1:10" x14ac:dyDescent="0.25">
@@ -14645,8 +14658,8 @@
         <v>0.50684931499999997</v>
       </c>
       <c r="J317">
-        <f t="shared" si="7"/>
-        <v>0.42351598166666665</v>
+        <f t="shared" si="12"/>
+        <v>0.84018264833333323</v>
       </c>
     </row>
     <row r="318" spans="1:10" x14ac:dyDescent="0.25">
@@ -14678,8 +14691,8 @@
         <v>0.50684931499999997</v>
       </c>
       <c r="J318">
-        <f t="shared" si="7"/>
-        <v>0.42351598166666665</v>
+        <f t="shared" si="12"/>
+        <v>0.84018264833333323</v>
       </c>
     </row>
     <row r="319" spans="1:10" x14ac:dyDescent="0.25">
@@ -14711,8 +14724,8 @@
         <v>0.80821917799999998</v>
       </c>
       <c r="J319">
-        <f t="shared" si="7"/>
-        <v>0.72488584466666661</v>
+        <f t="shared" si="12"/>
+        <v>0.14155251133333335</v>
       </c>
     </row>
     <row r="320" spans="1:10" x14ac:dyDescent="0.25">
@@ -14744,8 +14757,8 @@
         <v>0.80821917799999998</v>
       </c>
       <c r="J320">
-        <f t="shared" si="7"/>
-        <v>0.72488584466666661</v>
+        <f t="shared" si="12"/>
+        <v>0.14155251133333335</v>
       </c>
     </row>
     <row r="321" spans="1:10" x14ac:dyDescent="0.25">
@@ -14777,8 +14790,8 @@
         <v>0.80821917799999998</v>
       </c>
       <c r="J321">
-        <f t="shared" si="7"/>
-        <v>0.72488584466666661</v>
+        <f t="shared" si="12"/>
+        <v>0.14155251133333335</v>
       </c>
     </row>
     <row r="322" spans="1:10" x14ac:dyDescent="0.25">
@@ -14810,8 +14823,8 @@
         <v>0.89315068500000006</v>
       </c>
       <c r="J322">
-        <f t="shared" si="7"/>
-        <v>0.80981735166666668</v>
+        <f t="shared" si="12"/>
+        <v>0.22648401833333343</v>
       </c>
     </row>
     <row r="323" spans="1:10" x14ac:dyDescent="0.25">
@@ -14843,8 +14856,8 @@
         <v>0.89315068500000006</v>
       </c>
       <c r="J323">
-        <f t="shared" ref="J323:J339" si="8">IF(A323="R. diluvianum", I323, IF(A323="A. incurva", MOD(I323-4/12, 1), MOD(I323-1/12, 1)))</f>
-        <v>0.80981735166666668</v>
+        <f t="shared" ref="J323:J339" si="13">IF(A323="R. diluvianum", MOD(I323+5/12, 1), IF(A323="A. incurva", MOD(I323+1/12, 1), MOD(I323+4/12, 1)))</f>
+        <v>0.22648401833333343</v>
       </c>
     </row>
     <row r="324" spans="1:10" x14ac:dyDescent="0.25">
@@ -14876,8 +14889,8 @@
         <v>0.89315068500000006</v>
       </c>
       <c r="J324">
-        <f t="shared" si="8"/>
-        <v>0.80981735166666668</v>
+        <f t="shared" si="13"/>
+        <v>0.22648401833333343</v>
       </c>
     </row>
     <row r="325" spans="1:10" x14ac:dyDescent="0.25">
@@ -14909,8 +14922,8 @@
         <v>0.95068493200000004</v>
       </c>
       <c r="J325">
-        <f t="shared" si="8"/>
-        <v>0.86735159866666667</v>
+        <f t="shared" si="13"/>
+        <v>0.28401826533333341</v>
       </c>
     </row>
     <row r="326" spans="1:10" x14ac:dyDescent="0.25">
@@ -14942,8 +14955,8 @@
         <v>0.95068493200000004</v>
       </c>
       <c r="J326">
-        <f t="shared" si="8"/>
-        <v>0.86735159866666667</v>
+        <f t="shared" si="13"/>
+        <v>0.28401826533333341</v>
       </c>
     </row>
     <row r="327" spans="1:10" x14ac:dyDescent="0.25">
@@ -14975,8 +14988,8 @@
         <v>0.95068493200000004</v>
       </c>
       <c r="J327">
-        <f t="shared" si="8"/>
-        <v>0.86735159866666667</v>
+        <f t="shared" si="13"/>
+        <v>0.28401826533333341</v>
       </c>
     </row>
     <row r="328" spans="1:10" x14ac:dyDescent="0.25">
@@ -15008,8 +15021,8 @@
         <v>0</v>
       </c>
       <c r="J328">
-        <f t="shared" si="8"/>
-        <v>0.91666666666666663</v>
+        <f t="shared" si="13"/>
+        <v>0.33333333333333331</v>
       </c>
     </row>
     <row r="329" spans="1:10" x14ac:dyDescent="0.25">
@@ -15041,8 +15054,8 @@
         <v>0</v>
       </c>
       <c r="J329">
-        <f t="shared" si="8"/>
-        <v>0.91666666666666663</v>
+        <f t="shared" si="13"/>
+        <v>0.33333333333333331</v>
       </c>
     </row>
     <row r="330" spans="1:10" x14ac:dyDescent="0.25">
@@ -15074,8 +15087,8 @@
         <v>0</v>
       </c>
       <c r="J330">
-        <f t="shared" si="8"/>
-        <v>0.91666666666666663</v>
+        <f t="shared" si="13"/>
+        <v>0.33333333333333331</v>
       </c>
     </row>
     <row r="331" spans="1:10" x14ac:dyDescent="0.25">
@@ -15107,8 +15120,8 @@
         <v>4.1095890000000003E-2</v>
       </c>
       <c r="J331">
-        <f t="shared" si="8"/>
-        <v>0.95776255666666665</v>
+        <f t="shared" si="13"/>
+        <v>0.37442922333333334</v>
       </c>
     </row>
     <row r="332" spans="1:10" x14ac:dyDescent="0.25">
@@ -15140,8 +15153,8 @@
         <v>4.1095890000000003E-2</v>
       </c>
       <c r="J332">
-        <f t="shared" si="8"/>
-        <v>0.95776255666666665</v>
+        <f t="shared" si="13"/>
+        <v>0.37442922333333334</v>
       </c>
     </row>
     <row r="333" spans="1:10" x14ac:dyDescent="0.25">
@@ -15173,8 +15186,8 @@
         <v>4.1095890000000003E-2</v>
       </c>
       <c r="J333">
-        <f t="shared" si="8"/>
-        <v>0.95776255666666665</v>
+        <f t="shared" si="13"/>
+        <v>0.37442922333333334</v>
       </c>
     </row>
     <row r="334" spans="1:10" x14ac:dyDescent="0.25">
@@ -15206,8 +15219,8 @@
         <v>8.2191781000000005E-2</v>
       </c>
       <c r="J334">
-        <f t="shared" si="8"/>
-        <v>0.99885844766666665</v>
+        <f t="shared" si="13"/>
+        <v>0.41552511433333333</v>
       </c>
     </row>
     <row r="335" spans="1:10" x14ac:dyDescent="0.25">
@@ -15239,8 +15252,8 @@
         <v>8.2191781000000005E-2</v>
       </c>
       <c r="J335">
-        <f t="shared" si="8"/>
-        <v>0.99885844766666665</v>
+        <f t="shared" si="13"/>
+        <v>0.41552511433333333</v>
       </c>
     </row>
     <row r="336" spans="1:10" x14ac:dyDescent="0.25">
@@ -15272,8 +15285,8 @@
         <v>8.2191781000000005E-2</v>
       </c>
       <c r="J336">
-        <f t="shared" si="8"/>
-        <v>0.99885844766666665</v>
+        <f t="shared" si="13"/>
+        <v>0.41552511433333333</v>
       </c>
     </row>
     <row r="337" spans="1:10" x14ac:dyDescent="0.25">
@@ -15305,8 +15318,8 @@
         <v>0.120547945</v>
       </c>
       <c r="J337">
-        <f t="shared" si="8"/>
-        <v>3.7214611666666675E-2</v>
+        <f t="shared" si="13"/>
+        <v>0.4538812783333333</v>
       </c>
     </row>
     <row r="338" spans="1:10" x14ac:dyDescent="0.25">
@@ -15338,8 +15351,8 @@
         <v>0.16164383600000001</v>
       </c>
       <c r="J338">
-        <f t="shared" si="8"/>
-        <v>7.8310502666666684E-2</v>
+        <f t="shared" si="13"/>
+        <v>0.49497716933333336</v>
       </c>
     </row>
     <row r="339" spans="1:10" x14ac:dyDescent="0.25">
@@ -15371,8 +15384,8 @@
         <v>0.2</v>
       </c>
       <c r="J339">
-        <f t="shared" si="8"/>
-        <v>0.11666666666666668</v>
+        <f t="shared" si="13"/>
+        <v>0.53333333333333333</v>
       </c>
     </row>
   </sheetData>

</xml_diff>